<commit_message>
Updated tidsrapport to week 37
</commit_message>
<xml_diff>
--- a/tidsrapport/tidsrapportering3.xlsx
+++ b/tidsrapport/tidsrapportering3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehaagse\Desktop\code_snippets\tidsrapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CD35C7-E1BD-442F-A804-5EB8F7436A71}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90743323-0A77-411E-BB94-0A2976052428}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016 old" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6430" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6443" uniqueCount="316">
   <si>
     <t>vecka 38</t>
   </si>
@@ -980,6 +980,12 @@
   <si>
     <t>Ayleen tandläkare</t>
   </si>
+  <si>
+    <t>sum md:</t>
+  </si>
+  <si>
+    <t>reported --&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -1328,7 +1334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1521,6 +1527,8 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23256,10 +23264,10 @@
   <dimension ref="A1:AK723"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C678" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C663" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S684" sqref="S684"/>
+      <selection pane="bottomRight" activeCell="AJ680" sqref="AJ680"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58315,6 +58323,9 @@
       <c r="AB644" t="s">
         <v>300</v>
       </c>
+      <c r="AC644" t="s">
+        <v>314</v>
+      </c>
       <c r="AE644" s="92"/>
     </row>
     <row r="645" spans="1:33" x14ac:dyDescent="0.35">
@@ -58384,6 +58395,10 @@
       <c r="AB645" s="10">
         <f>AB638+Z645</f>
         <v>-2.036666666666676</v>
+      </c>
+      <c r="AC645" s="10">
+        <f>AC638+Y645</f>
+        <v>40.266666666666673</v>
       </c>
     </row>
     <row r="646" spans="1:33" x14ac:dyDescent="0.35">
@@ -58428,7 +58443,10 @@
       <c r="Z646" s="66"/>
       <c r="AA646" s="66"/>
       <c r="AB646" s="69"/>
-      <c r="AC646" s="58"/>
+      <c r="AC646" s="132">
+        <f>AC639+Y646</f>
+        <v>40</v>
+      </c>
       <c r="AD646" s="124"/>
       <c r="AE646" s="58"/>
       <c r="AF646" s="58"/>
@@ -58706,6 +58724,9 @@
       <c r="AB651" t="s">
         <v>300</v>
       </c>
+      <c r="AC651" t="s">
+        <v>314</v>
+      </c>
       <c r="AE651" s="92"/>
     </row>
     <row r="652" spans="1:33" x14ac:dyDescent="0.35">
@@ -58773,6 +58794,10 @@
       <c r="AB652" s="10">
         <f>AB645+Z652</f>
         <v>-10.353333333333346</v>
+      </c>
+      <c r="AC652" s="10">
+        <f>AC645+Y652</f>
+        <v>71.95</v>
       </c>
     </row>
     <row r="653" spans="1:33" x14ac:dyDescent="0.35">
@@ -58817,7 +58842,10 @@
       <c r="Z653" s="66"/>
       <c r="AA653" s="66"/>
       <c r="AB653" s="69"/>
-      <c r="AC653" s="58"/>
+      <c r="AC653" s="132">
+        <f>AC646+Y653</f>
+        <v>72</v>
+      </c>
       <c r="AD653" s="124"/>
       <c r="AE653" s="58"/>
       <c r="AF653" s="58"/>
@@ -59047,6 +59075,9 @@
       <c r="AB658" t="s">
         <v>300</v>
       </c>
+      <c r="AC658" t="s">
+        <v>314</v>
+      </c>
       <c r="AE658" s="92"/>
     </row>
     <row r="659" spans="1:33" x14ac:dyDescent="0.35">
@@ -59102,6 +59133,10 @@
       <c r="AB659" s="10">
         <f>AB652+Z659</f>
         <v>-50.353333333333346</v>
+      </c>
+      <c r="AC659" s="10">
+        <f>AC652+Y659</f>
+        <v>71.95</v>
       </c>
     </row>
     <row r="660" spans="1:33" x14ac:dyDescent="0.35">
@@ -59146,7 +59181,10 @@
       <c r="Z660" s="66"/>
       <c r="AA660" s="66"/>
       <c r="AB660" s="69"/>
-      <c r="AC660" s="58"/>
+      <c r="AC660" s="132">
+        <f>AC653+Y660</f>
+        <v>72</v>
+      </c>
       <c r="AD660" s="124"/>
       <c r="AE660" s="58"/>
       <c r="AF660" s="58"/>
@@ -59435,6 +59473,9 @@
       <c r="AB665" t="s">
         <v>300</v>
       </c>
+      <c r="AC665" t="s">
+        <v>314</v>
+      </c>
       <c r="AE665" s="92"/>
     </row>
     <row r="666" spans="1:33" x14ac:dyDescent="0.35">
@@ -59504,6 +59545,10 @@
       <c r="AB666" s="10">
         <f>AB659+Z666</f>
         <v>-58.586666666666687</v>
+      </c>
+      <c r="AC666" s="13">
+        <f>Y666</f>
+        <v>31.766666666666662</v>
       </c>
     </row>
     <row r="667" spans="1:33" x14ac:dyDescent="0.35">
@@ -59548,7 +59593,10 @@
       <c r="Z667" s="66"/>
       <c r="AA667" s="66"/>
       <c r="AB667" s="69"/>
-      <c r="AC667" s="58"/>
+      <c r="AC667" s="133">
+        <f>Y667</f>
+        <v>32</v>
+      </c>
       <c r="AD667" s="124"/>
       <c r="AE667" s="58"/>
       <c r="AF667" s="58"/>
@@ -59834,6 +59882,9 @@
       <c r="AB672" t="s">
         <v>300</v>
       </c>
+      <c r="AC672" t="s">
+        <v>314</v>
+      </c>
       <c r="AE672" s="92"/>
     </row>
     <row r="673" spans="1:33" x14ac:dyDescent="0.35">
@@ -59889,6 +59940,10 @@
       <c r="AB673" s="10">
         <f>AB666+Z673</f>
         <v>-57.686666666666682</v>
+      </c>
+      <c r="AC673" s="10">
+        <f>AC666+Y673</f>
+        <v>64.666666666666671</v>
       </c>
     </row>
     <row r="674" spans="1:33" x14ac:dyDescent="0.35">
@@ -59933,7 +59988,10 @@
       <c r="Z674" s="66"/>
       <c r="AA674" s="66"/>
       <c r="AB674" s="69"/>
-      <c r="AC674" s="58"/>
+      <c r="AC674" s="132">
+        <f>AC667+Y674</f>
+        <v>65</v>
+      </c>
       <c r="AD674" s="124"/>
       <c r="AE674" s="58"/>
       <c r="AF674" s="58"/>
@@ -60219,6 +60277,9 @@
       <c r="AB679" t="s">
         <v>300</v>
       </c>
+      <c r="AC679" t="s">
+        <v>314</v>
+      </c>
       <c r="AE679" s="92"/>
     </row>
     <row r="680" spans="1:33" x14ac:dyDescent="0.35">
@@ -60288,6 +60349,10 @@
       <c r="AB680" s="10">
         <f>AB673+Z680</f>
         <v>-58.353333333333353</v>
+      </c>
+      <c r="AC680" s="10">
+        <f>AC673+Y680</f>
+        <v>104</v>
       </c>
     </row>
     <row r="681" spans="1:33" x14ac:dyDescent="0.35">
@@ -60332,7 +60397,10 @@
       <c r="Z681" s="66"/>
       <c r="AA681" s="66"/>
       <c r="AB681" s="69"/>
-      <c r="AC681" s="58"/>
+      <c r="AC681" s="132">
+        <f>AC674+Y681</f>
+        <v>104.5</v>
+      </c>
       <c r="AD681" s="124"/>
       <c r="AE681" s="58"/>
       <c r="AF681" s="58"/>
@@ -60620,6 +60688,9 @@
       <c r="AB686" t="s">
         <v>300</v>
       </c>
+      <c r="AC686" t="s">
+        <v>314</v>
+      </c>
       <c r="AE686" s="92"/>
     </row>
     <row r="687" spans="1:33" x14ac:dyDescent="0.35">
@@ -60687,6 +60758,10 @@
       <c r="AB687" s="10">
         <f>AB680+Z687</f>
         <v>-60.453333333333347</v>
+      </c>
+      <c r="AC687" s="10">
+        <f>AC681+Y687</f>
+        <v>142.4</v>
       </c>
     </row>
     <row r="688" spans="1:33" x14ac:dyDescent="0.35">
@@ -60731,7 +60806,10 @@
       <c r="Z688" s="66"/>
       <c r="AA688" s="66"/>
       <c r="AB688" s="69"/>
-      <c r="AC688" s="58"/>
+      <c r="AC688" s="132">
+        <f>AC681+Y688</f>
+        <v>142.5</v>
+      </c>
       <c r="AD688" s="124"/>
       <c r="AE688" s="58"/>
       <c r="AF688" s="58"/>
@@ -60742,7 +60820,7 @@
         <v>43716</v>
       </c>
       <c r="B689" s="6" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="C689" s="1"/>
       <c r="D689" s="1"/>
@@ -60796,8 +60874,20 @@
         <v>1</v>
       </c>
       <c r="D690" s="1"/>
+      <c r="E690">
+        <v>8</v>
+      </c>
+      <c r="F690">
+        <v>40</v>
+      </c>
       <c r="G690" s="79" t="s">
         <v>6</v>
+      </c>
+      <c r="H690">
+        <v>16</v>
+      </c>
+      <c r="I690">
+        <v>28</v>
       </c>
       <c r="J690" s="82" t="s">
         <v>17</v>
@@ -60811,7 +60901,7 @@
       <c r="S690" s="4"/>
       <c r="T690" s="10">
         <f>(I690/60+H690)-(F690/60+E690)</f>
-        <v>0</v>
+        <v>7.7999999999999989</v>
       </c>
       <c r="U690" s="10">
         <f>(O690/60+N690)-(L690/60+K690)</f>
@@ -60820,9 +60910,11 @@
       <c r="V690" s="10"/>
       <c r="W690" s="11">
         <f>T690+U690-Q690*0.5+V690</f>
-        <v>0</v>
-      </c>
-      <c r="X690" s="106"/>
+        <v>7.7999999999999989</v>
+      </c>
+      <c r="X690" s="106">
+        <v>9</v>
+      </c>
       <c r="AC690" s="8"/>
     </row>
     <row r="691" spans="1:33" x14ac:dyDescent="0.35">
@@ -60834,9 +60926,21 @@
         <v>2</v>
       </c>
       <c r="D691" s="1"/>
+      <c r="E691">
+        <v>8</v>
+      </c>
+      <c r="F691">
+        <v>25</v>
+      </c>
       <c r="G691" s="79" t="s">
         <v>6</v>
       </c>
+      <c r="H691">
+        <v>17</v>
+      </c>
+      <c r="I691">
+        <v>15</v>
+      </c>
       <c r="J691" s="82" t="s">
         <v>17</v>
       </c>
@@ -60844,12 +60948,14 @@
         <v>6</v>
       </c>
       <c r="P691" s="1"/>
-      <c r="Q691" s="3"/>
+      <c r="Q691" s="3">
+        <v>1</v>
+      </c>
       <c r="R691" s="5"/>
       <c r="S691" s="4"/>
       <c r="T691" s="10">
         <f>(I691/60+H691)-(F691/60+E691)</f>
-        <v>0</v>
+        <v>8.8333333333333339</v>
       </c>
       <c r="U691" s="10">
         <f>(O691/60+N691)-(L691/60+K691)</f>
@@ -60858,9 +60964,11 @@
       <c r="V691" s="10"/>
       <c r="W691" s="11">
         <f>T691+U691-Q691*0.5+V691</f>
-        <v>0</v>
-      </c>
-      <c r="X691" s="10"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="X691" s="10">
+        <v>9</v>
+      </c>
       <c r="Z691" t="s">
         <v>258</v>
       </c>
@@ -60874,8 +60982,20 @@
         <v>3</v>
       </c>
       <c r="D692" s="1"/>
+      <c r="E692">
+        <v>8</v>
+      </c>
+      <c r="F692">
+        <v>10</v>
+      </c>
       <c r="G692" s="79" t="s">
         <v>6</v>
+      </c>
+      <c r="H692">
+        <v>19</v>
+      </c>
+      <c r="I692">
+        <v>20</v>
       </c>
       <c r="J692" s="82" t="s">
         <v>17</v>
@@ -60889,7 +61009,7 @@
       <c r="S692" s="4"/>
       <c r="T692" s="10">
         <f>(I692/60+H692)-(F692/60+E692)</f>
-        <v>0</v>
+        <v>11.166666666666666</v>
       </c>
       <c r="U692" s="10">
         <f>(O692/60+N692)-(L692/60+K692)</f>
@@ -60898,9 +61018,11 @@
       <c r="V692" s="10"/>
       <c r="W692" s="11">
         <f>T692+U692-Q692*0.5+V692</f>
-        <v>0</v>
-      </c>
-      <c r="X692" s="10"/>
+        <v>11.166666666666666</v>
+      </c>
+      <c r="X692" s="10">
+        <v>9</v>
+      </c>
       <c r="Z692" s="74">
         <v>0</v>
       </c>
@@ -60914,8 +61036,20 @@
         <v>4</v>
       </c>
       <c r="D693" s="1"/>
+      <c r="E693">
+        <v>8</v>
+      </c>
+      <c r="F693">
+        <v>2</v>
+      </c>
       <c r="G693" s="79" t="s">
         <v>6</v>
+      </c>
+      <c r="H693">
+        <v>15</v>
+      </c>
+      <c r="I693">
+        <v>40</v>
       </c>
       <c r="J693" s="82" t="s">
         <v>17</v>
@@ -60929,7 +61063,7 @@
       <c r="S693" s="4"/>
       <c r="T693" s="10">
         <f>(I693/60+H693)-(F693/60+E693)</f>
-        <v>0</v>
+        <v>7.6333333333333329</v>
       </c>
       <c r="U693" s="10">
         <f>(O693/60+N693)-(L693/60+K693)</f>
@@ -60938,9 +61072,11 @@
       <c r="V693" s="10"/>
       <c r="W693" s="11">
         <f>T693+U693-Q693*0.5+V693</f>
-        <v>0</v>
-      </c>
-      <c r="X693" s="10"/>
+        <v>7.6333333333333329</v>
+      </c>
+      <c r="X693" s="10">
+        <v>8</v>
+      </c>
       <c r="Y693" t="s">
         <v>11</v>
       </c>
@@ -60952,6 +61088,9 @@
       </c>
       <c r="AB693" t="s">
         <v>300</v>
+      </c>
+      <c r="AC693" t="s">
+        <v>314</v>
       </c>
       <c r="AE693" s="92"/>
     </row>
@@ -60964,8 +61103,20 @@
         <v>5</v>
       </c>
       <c r="D694" s="1"/>
+      <c r="E694">
+        <v>8</v>
+      </c>
+      <c r="F694">
+        <v>23</v>
+      </c>
       <c r="G694" s="79" t="s">
         <v>6</v>
+      </c>
+      <c r="H694">
+        <v>16</v>
+      </c>
+      <c r="I694">
+        <v>30</v>
       </c>
       <c r="J694" s="82" t="s">
         <v>17</v>
@@ -60979,7 +61130,7 @@
       <c r="S694" s="4"/>
       <c r="T694" s="10">
         <f>(I694/60+H694)-(F694/60+E694)</f>
-        <v>0</v>
+        <v>8.1166666666666671</v>
       </c>
       <c r="U694" s="10">
         <f>(O694/60+N694)-(L694/60+K694)</f>
@@ -60988,24 +61139,30 @@
       <c r="V694" s="10"/>
       <c r="W694" s="11">
         <f>T694+U694-Q694*0.5+V694</f>
-        <v>0</v>
-      </c>
-      <c r="X694" s="10"/>
+        <v>8.1166666666666671</v>
+      </c>
+      <c r="X694" s="10">
+        <v>8</v>
+      </c>
       <c r="Y694" s="12">
         <f>SUM(W690:W694)</f>
-        <v>0</v>
+        <v>43.05</v>
       </c>
       <c r="Z694" s="10">
         <f>Y694-(8*(5-Z692))+SUM(S690:S694)*8</f>
-        <v>-40</v>
+        <v>3.0499999999999972</v>
       </c>
       <c r="AA694" s="10">
         <f>AA687+Z694</f>
-        <v>-104.1</v>
+        <v>-61.05</v>
       </c>
       <c r="AB694" s="10">
         <f>AB687+Z694</f>
-        <v>-100.45333333333335</v>
+        <v>-57.40333333333335</v>
+      </c>
+      <c r="AC694" s="10">
+        <f>AC687+Y694</f>
+        <v>185.45</v>
       </c>
     </row>
     <row r="695" spans="1:33" x14ac:dyDescent="0.35">
@@ -61042,15 +61199,20 @@
       <c r="U695" s="71"/>
       <c r="V695" s="71"/>
       <c r="W695" s="72"/>
-      <c r="X695" s="68"/>
+      <c r="X695" s="68" t="s">
+        <v>315</v>
+      </c>
       <c r="Y695" s="120">
         <f>SUM(X690:X694)</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="Z695" s="66"/>
       <c r="AA695" s="66"/>
       <c r="AB695" s="69"/>
-      <c r="AC695" s="58"/>
+      <c r="AC695" s="132">
+        <f>AC688+Y695</f>
+        <v>185.5</v>
+      </c>
       <c r="AD695" s="124"/>
       <c r="AE695" s="58"/>
       <c r="AF695" s="58"/>
@@ -61272,6 +61434,9 @@
       <c r="AB700" t="s">
         <v>300</v>
       </c>
+      <c r="AC700" t="s">
+        <v>314</v>
+      </c>
       <c r="AE700" s="92"/>
     </row>
     <row r="701" spans="1:33" x14ac:dyDescent="0.35">
@@ -61320,11 +61485,15 @@
       </c>
       <c r="AA701" s="10">
         <f>AA694+Z701</f>
-        <v>-144.1</v>
+        <v>-101.05</v>
       </c>
       <c r="AB701" s="10">
         <f>AB694+Z701</f>
-        <v>-140.45333333333335</v>
+        <v>-97.40333333333335</v>
+      </c>
+      <c r="AC701" s="10">
+        <f>AC694+Y701</f>
+        <v>185.45</v>
       </c>
     </row>
     <row r="702" spans="1:33" x14ac:dyDescent="0.35">
@@ -61369,7 +61538,10 @@
       <c r="Z702" s="66"/>
       <c r="AA702" s="66"/>
       <c r="AB702" s="69"/>
-      <c r="AC702" s="58"/>
+      <c r="AC702" s="132">
+        <f>AC695+Y702</f>
+        <v>185.5</v>
+      </c>
       <c r="AD702" s="124"/>
       <c r="AE702" s="58"/>
       <c r="AF702" s="58"/>
@@ -61591,6 +61763,9 @@
       <c r="AB707" t="s">
         <v>300</v>
       </c>
+      <c r="AC707" t="s">
+        <v>314</v>
+      </c>
       <c r="AE707" s="92"/>
     </row>
     <row r="708" spans="1:33" x14ac:dyDescent="0.35">
@@ -61639,11 +61814,15 @@
       </c>
       <c r="AA708" s="10">
         <f>AA701+Z708</f>
-        <v>-184.1</v>
+        <v>-141.05000000000001</v>
       </c>
       <c r="AB708" s="10">
         <f>AB701+Z708</f>
-        <v>-180.45333333333335</v>
+        <v>-137.40333333333336</v>
+      </c>
+      <c r="AC708" s="10">
+        <f>AC701+Y708</f>
+        <v>185.45</v>
       </c>
     </row>
     <row r="709" spans="1:33" x14ac:dyDescent="0.35">
@@ -61688,7 +61867,10 @@
       <c r="Z709" s="66"/>
       <c r="AA709" s="66"/>
       <c r="AB709" s="69"/>
-      <c r="AC709" s="58"/>
+      <c r="AC709" s="132">
+        <f>AC702+Y709</f>
+        <v>185.5</v>
+      </c>
       <c r="AD709" s="124"/>
       <c r="AE709" s="58"/>
       <c r="AF709" s="58"/>
@@ -61910,6 +62092,9 @@
       <c r="AB714" t="s">
         <v>300</v>
       </c>
+      <c r="AC714" t="s">
+        <v>314</v>
+      </c>
       <c r="AE714" s="92"/>
     </row>
     <row r="715" spans="1:33" x14ac:dyDescent="0.35">
@@ -61958,11 +62143,15 @@
       </c>
       <c r="AA715" s="10">
         <f>AA708+Z715</f>
-        <v>-224.1</v>
+        <v>-181.05</v>
       </c>
       <c r="AB715" s="10">
         <f>AB708+Z715</f>
-        <v>-220.45333333333335</v>
+        <v>-177.40333333333336</v>
+      </c>
+      <c r="AC715" s="10">
+        <f>AC708+Y715</f>
+        <v>185.45</v>
       </c>
     </row>
     <row r="716" spans="1:33" x14ac:dyDescent="0.35">
@@ -62007,7 +62196,10 @@
       <c r="Z716" s="66"/>
       <c r="AA716" s="66"/>
       <c r="AB716" s="69"/>
-      <c r="AC716" s="58"/>
+      <c r="AC716" s="132">
+        <f>AC709+Y716</f>
+        <v>185.5</v>
+      </c>
       <c r="AD716" s="124"/>
       <c r="AE716" s="58"/>
       <c r="AF716" s="58"/>
@@ -62229,6 +62421,9 @@
       <c r="AB721" t="s">
         <v>300</v>
       </c>
+      <c r="AC721" t="s">
+        <v>314</v>
+      </c>
       <c r="AE721" s="92"/>
     </row>
     <row r="722" spans="1:33" x14ac:dyDescent="0.35">
@@ -62277,11 +62472,15 @@
       </c>
       <c r="AA722" s="10">
         <f>AA715+Z722</f>
-        <v>-264.10000000000002</v>
+        <v>-221.05</v>
       </c>
       <c r="AB722" s="10">
         <f>AB715+Z722</f>
-        <v>-260.45333333333338</v>
+        <v>-217.40333333333336</v>
+      </c>
+      <c r="AC722" s="10">
+        <f>AC715+Y722</f>
+        <v>185.45</v>
       </c>
     </row>
     <row r="723" spans="1:33" x14ac:dyDescent="0.35">
@@ -62326,7 +62525,10 @@
       <c r="Z723" s="66"/>
       <c r="AA723" s="66"/>
       <c r="AB723" s="69"/>
-      <c r="AC723" s="58"/>
+      <c r="AC723" s="132">
+        <f>AC716+Y723</f>
+        <v>185.5</v>
+      </c>
       <c r="AD723" s="124"/>
       <c r="AE723" s="58"/>
       <c r="AF723" s="58"/>
@@ -62334,48 +62536,6 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="E437:I437"/>
-    <mergeCell ref="K437:O437"/>
-    <mergeCell ref="E430:I430"/>
-    <mergeCell ref="K430:O430"/>
-    <mergeCell ref="E409:I409"/>
-    <mergeCell ref="K409:O409"/>
-    <mergeCell ref="E416:I416"/>
-    <mergeCell ref="K416:O416"/>
-    <mergeCell ref="E423:I423"/>
-    <mergeCell ref="K423:O423"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="E304:I304"/>
-    <mergeCell ref="K304:O304"/>
-    <mergeCell ref="E283:I283"/>
-    <mergeCell ref="K283:O283"/>
-    <mergeCell ref="E276:I276"/>
-    <mergeCell ref="K276:O276"/>
-    <mergeCell ref="E269:I269"/>
-    <mergeCell ref="K269:O269"/>
-    <mergeCell ref="E262:I262"/>
-    <mergeCell ref="K262:O262"/>
-    <mergeCell ref="E339:I339"/>
-    <mergeCell ref="K339:O339"/>
-    <mergeCell ref="E290:I290"/>
-    <mergeCell ref="K290:O290"/>
-    <mergeCell ref="E311:I311"/>
-    <mergeCell ref="K311:O311"/>
-    <mergeCell ref="E318:I318"/>
-    <mergeCell ref="K318:O318"/>
-    <mergeCell ref="E325:I325"/>
-    <mergeCell ref="K325:O325"/>
-    <mergeCell ref="E297:I297"/>
-    <mergeCell ref="K297:O297"/>
-    <mergeCell ref="E332:I332"/>
-    <mergeCell ref="K332:O332"/>
-    <mergeCell ref="E346:I346"/>
-    <mergeCell ref="K346:O346"/>
-    <mergeCell ref="E353:I353"/>
-    <mergeCell ref="K353:O353"/>
-    <mergeCell ref="E360:I360"/>
-    <mergeCell ref="K360:O360"/>
     <mergeCell ref="E444:I444"/>
     <mergeCell ref="K444:O444"/>
     <mergeCell ref="E451:I451"/>
@@ -62392,6 +62552,48 @@
     <mergeCell ref="K395:O395"/>
     <mergeCell ref="E402:I402"/>
     <mergeCell ref="K402:O402"/>
+    <mergeCell ref="E346:I346"/>
+    <mergeCell ref="K346:O346"/>
+    <mergeCell ref="E353:I353"/>
+    <mergeCell ref="K353:O353"/>
+    <mergeCell ref="E360:I360"/>
+    <mergeCell ref="K360:O360"/>
+    <mergeCell ref="E339:I339"/>
+    <mergeCell ref="K339:O339"/>
+    <mergeCell ref="E290:I290"/>
+    <mergeCell ref="K290:O290"/>
+    <mergeCell ref="E311:I311"/>
+    <mergeCell ref="K311:O311"/>
+    <mergeCell ref="E318:I318"/>
+    <mergeCell ref="K318:O318"/>
+    <mergeCell ref="E325:I325"/>
+    <mergeCell ref="K325:O325"/>
+    <mergeCell ref="E297:I297"/>
+    <mergeCell ref="K297:O297"/>
+    <mergeCell ref="E332:I332"/>
+    <mergeCell ref="K332:O332"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="E304:I304"/>
+    <mergeCell ref="K304:O304"/>
+    <mergeCell ref="E283:I283"/>
+    <mergeCell ref="K283:O283"/>
+    <mergeCell ref="E276:I276"/>
+    <mergeCell ref="K276:O276"/>
+    <mergeCell ref="E269:I269"/>
+    <mergeCell ref="K269:O269"/>
+    <mergeCell ref="E262:I262"/>
+    <mergeCell ref="K262:O262"/>
+    <mergeCell ref="E437:I437"/>
+    <mergeCell ref="K437:O437"/>
+    <mergeCell ref="E430:I430"/>
+    <mergeCell ref="K430:O430"/>
+    <mergeCell ref="E409:I409"/>
+    <mergeCell ref="K409:O409"/>
+    <mergeCell ref="E416:I416"/>
+    <mergeCell ref="K416:O416"/>
+    <mergeCell ref="E423:I423"/>
+    <mergeCell ref="K423:O423"/>
   </mergeCells>
   <conditionalFormatting sqref="Y216">
     <cfRule type="colorScale" priority="81">
@@ -62403,7 +62605,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y307 Y209 Y300 Y293 Y286 Y279 Y272 Y265 Y258 Y251 Y244 Y237 Y230 Y223 Y172 Y178 Y184 Y190 Y196 Y202">
+  <conditionalFormatting sqref="Y209 Y307 Y300 Y293 Y286 Y279 Y272 Y265 Y258 Y251 Y244 Y237 Y230 Y223 Y172 Y178 Y184 Y190 Y196 Y202">
     <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -62423,7 +62625,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD309 AD218 AD225 AD232 AD239 AD246 AD253 AD260 AD266 AD281 AD288 AD295 AD302">
+  <conditionalFormatting sqref="AD218 AD309 AD225 AD232 AD239 AD246 AD253 AD260 AD266 AD281 AD288 AD295 AD302">
     <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Updated the time report to week 45 + Formatting
</commit_message>
<xml_diff>
--- a/tidsrapport/tidsrapportering3.xlsx
+++ b/tidsrapport/tidsrapportering3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehaagse\Desktop\code_snippets\tidsrapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACC3C4C-A932-454B-ADE2-35B890373FF3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF637DAF-D7BD-4778-A156-7BD538CA8AC4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016 old" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6805" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6817" uniqueCount="318">
   <si>
     <t>vecka 38</t>
   </si>
@@ -989,6 +989,9 @@
   <si>
     <t>1,5 hackaton</t>
   </si>
+  <si>
+    <t>Alice' tandläkare</t>
+  </si>
 </sst>
 </file>
 
@@ -23273,10 +23276,10 @@
   <dimension ref="A1:AK786"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C724" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C700" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="X725" sqref="X725"/>
+      <selection pane="bottomRight" activeCell="X721" sqref="X721"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23298,7 +23301,7 @@
     <col min="20" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="2.140625" customWidth="1"/>
     <col min="23" max="23" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" customWidth="1"/>
     <col min="25" max="25" width="10.5703125" customWidth="1"/>
     <col min="26" max="27" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8.7109375" style="99"/>
@@ -62637,7 +62640,9 @@
         <f>T720+U720-Q720*0.5+V720</f>
         <v>0</v>
       </c>
-      <c r="X720" s="10"/>
+      <c r="X720" s="10">
+        <v>0</v>
+      </c>
       <c r="Z720" s="74">
         <v>1</v>
       </c>
@@ -62825,7 +62830,9 @@
       </c>
       <c r="Z723" s="66"/>
       <c r="AA723" s="66"/>
-      <c r="AB723" s="69"/>
+      <c r="AB723" s="69" t="s">
+        <v>285</v>
+      </c>
       <c r="AC723" s="129">
         <f>AC716+Y723</f>
         <v>324</v>
@@ -63242,7 +63249,9 @@
       </c>
       <c r="Z730" s="66"/>
       <c r="AA730" s="66"/>
-      <c r="AB730" s="69"/>
+      <c r="AB730" s="69" t="s">
+        <v>285</v>
+      </c>
       <c r="AC730" s="129">
         <f>AC723+Y730</f>
         <v>364</v>
@@ -63649,7 +63658,9 @@
       </c>
       <c r="Z737" s="66"/>
       <c r="AA737" s="66"/>
-      <c r="AB737" s="69"/>
+      <c r="AB737" s="69" t="s">
+        <v>285</v>
+      </c>
       <c r="AC737" s="129">
         <f>AC730+Y737</f>
         <v>406.5</v>
@@ -63664,7 +63675,7 @@
         <v>43765</v>
       </c>
       <c r="B738" s="6" t="s">
-        <v>298</v>
+        <v>24</v>
       </c>
       <c r="C738" s="1"/>
       <c r="D738" s="1"/>
@@ -63713,7 +63724,9 @@
       <c r="A739" s="52">
         <v>43766</v>
       </c>
-      <c r="B739" s="9"/>
+      <c r="B739" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="C739" s="1" t="s">
         <v>1</v>
       </c>
@@ -63751,7 +63764,9 @@
       <c r="A740" s="52">
         <v>43767</v>
       </c>
-      <c r="B740" s="9"/>
+      <c r="B740" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="C740" s="1" t="s">
         <v>2</v>
       </c>
@@ -63791,7 +63806,9 @@
       <c r="A741" s="52">
         <v>43768</v>
       </c>
-      <c r="B741" s="9"/>
+      <c r="B741" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="C741" s="1" t="s">
         <v>3</v>
       </c>
@@ -63824,14 +63841,16 @@
       </c>
       <c r="X741" s="10"/>
       <c r="Z741" s="74">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="742" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A742" s="52">
         <v>43769</v>
       </c>
-      <c r="B742" s="9"/>
+      <c r="B742" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="C742" s="1" t="s">
         <v>4</v>
       </c>
@@ -63884,7 +63903,9 @@
       <c r="A743" s="52">
         <v>43770</v>
       </c>
-      <c r="B743" s="9"/>
+      <c r="B743" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="C743" s="1" t="s">
         <v>5</v>
       </c>
@@ -63922,15 +63943,15 @@
       </c>
       <c r="Z743" s="10">
         <f>Y743-(8*(5-Z741))+SUM(S739:S743)*8</f>
-        <v>-40</v>
+        <v>0</v>
       </c>
       <c r="AA743" s="10">
         <f>AA736+Z743</f>
-        <v>-111.7</v>
+        <v>-71.7</v>
       </c>
       <c r="AB743" s="10">
         <f>AB736+Z743</f>
-        <v>-108.05333333333336</v>
+        <v>-68.053333333333356</v>
       </c>
       <c r="AC743" s="10">
         <f>AC736+Y743</f>
@@ -63978,7 +63999,9 @@
       </c>
       <c r="Z744" s="66"/>
       <c r="AA744" s="66"/>
-      <c r="AB744" s="69"/>
+      <c r="AB744" s="69" t="s">
+        <v>285</v>
+      </c>
       <c r="AC744" s="129">
         <f>AC737+Y744</f>
         <v>406.5</v>
@@ -63993,7 +64016,7 @@
         <v>43772</v>
       </c>
       <c r="B745" s="6" t="s">
-        <v>298</v>
+        <v>25</v>
       </c>
       <c r="C745" s="1"/>
       <c r="D745" s="1"/>
@@ -64047,8 +64070,20 @@
         <v>1</v>
       </c>
       <c r="D746" s="1"/>
+      <c r="E746">
+        <v>8</v>
+      </c>
+      <c r="F746">
+        <v>33</v>
+      </c>
       <c r="G746" s="79" t="s">
         <v>6</v>
+      </c>
+      <c r="H746">
+        <v>15</v>
+      </c>
+      <c r="I746">
+        <v>31</v>
       </c>
       <c r="J746" s="82" t="s">
         <v>17</v>
@@ -64062,7 +64097,7 @@
       <c r="S746" s="4"/>
       <c r="T746" s="10">
         <f>(I746/60+H746)-(F746/60+E746)</f>
-        <v>0</v>
+        <v>6.9666666666666668</v>
       </c>
       <c r="U746" s="10">
         <f>(O746/60+N746)-(L746/60+K746)</f>
@@ -64071,9 +64106,11 @@
       <c r="V746" s="10"/>
       <c r="W746" s="11">
         <f>T746+U746-Q746*0.5+V746</f>
-        <v>0</v>
-      </c>
-      <c r="X746" s="106"/>
+        <v>6.9666666666666668</v>
+      </c>
+      <c r="X746" s="106">
+        <v>8</v>
+      </c>
       <c r="AC746" s="8"/>
     </row>
     <row r="747" spans="1:33" x14ac:dyDescent="0.25">
@@ -64085,9 +64122,21 @@
         <v>2</v>
       </c>
       <c r="D747" s="1"/>
+      <c r="E747">
+        <v>8</v>
+      </c>
+      <c r="F747">
+        <v>51</v>
+      </c>
       <c r="G747" s="79" t="s">
         <v>6</v>
       </c>
+      <c r="H747">
+        <v>17</v>
+      </c>
+      <c r="I747">
+        <v>15</v>
+      </c>
       <c r="J747" s="82" t="s">
         <v>17</v>
       </c>
@@ -64095,12 +64144,14 @@
         <v>6</v>
       </c>
       <c r="P747" s="1"/>
-      <c r="Q747" s="3"/>
+      <c r="Q747" s="3">
+        <v>2</v>
+      </c>
       <c r="R747" s="5"/>
       <c r="S747" s="4"/>
       <c r="T747" s="10">
         <f>(I747/60+H747)-(F747/60+E747)</f>
-        <v>0</v>
+        <v>8.4</v>
       </c>
       <c r="U747" s="10">
         <f>(O747/60+N747)-(L747/60+K747)</f>
@@ -64109,9 +64160,11 @@
       <c r="V747" s="10"/>
       <c r="W747" s="11">
         <f>T747+U747-Q747*0.5+V747</f>
-        <v>0</v>
-      </c>
-      <c r="X747" s="10"/>
+        <v>7.4</v>
+      </c>
+      <c r="X747" s="10">
+        <v>8</v>
+      </c>
       <c r="Z747" t="s">
         <v>258</v>
       </c>
@@ -64120,13 +64173,27 @@
       <c r="A748" s="52">
         <v>43775</v>
       </c>
-      <c r="B748" s="9"/>
+      <c r="B748" s="9" t="s">
+        <v>317</v>
+      </c>
       <c r="C748" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D748" s="1"/>
+      <c r="E748">
+        <v>8</v>
+      </c>
+      <c r="F748">
+        <v>27</v>
+      </c>
       <c r="G748" s="79" t="s">
         <v>6</v>
+      </c>
+      <c r="H748">
+        <v>14</v>
+      </c>
+      <c r="I748">
+        <v>50</v>
       </c>
       <c r="J748" s="82" t="s">
         <v>17</v>
@@ -64140,7 +64207,7 @@
       <c r="S748" s="4"/>
       <c r="T748" s="10">
         <f>(I748/60+H748)-(F748/60+E748)</f>
-        <v>0</v>
+        <v>6.3833333333333346</v>
       </c>
       <c r="U748" s="10">
         <f>(O748/60+N748)-(L748/60+K748)</f>
@@ -64149,9 +64216,11 @@
       <c r="V748" s="10"/>
       <c r="W748" s="11">
         <f>T748+U748-Q748*0.5+V748</f>
-        <v>0</v>
-      </c>
-      <c r="X748" s="10"/>
+        <v>6.3833333333333346</v>
+      </c>
+      <c r="X748" s="10">
+        <v>6</v>
+      </c>
       <c r="Z748" s="74">
         <v>0</v>
       </c>
@@ -64165,9 +64234,21 @@
         <v>4</v>
       </c>
       <c r="D749" s="1"/>
+      <c r="E749">
+        <v>8</v>
+      </c>
+      <c r="F749">
+        <v>41</v>
+      </c>
       <c r="G749" s="79" t="s">
         <v>6</v>
       </c>
+      <c r="H749">
+        <v>20</v>
+      </c>
+      <c r="I749">
+        <v>0</v>
+      </c>
       <c r="J749" s="82" t="s">
         <v>17</v>
       </c>
@@ -64175,12 +64256,14 @@
         <v>6</v>
       </c>
       <c r="P749" s="1"/>
-      <c r="Q749" s="3"/>
+      <c r="Q749" s="3">
+        <v>1</v>
+      </c>
       <c r="R749" s="5"/>
       <c r="S749" s="4"/>
       <c r="T749" s="10">
         <f>(I749/60+H749)-(F749/60+E749)</f>
-        <v>0</v>
+        <v>11.316666666666666</v>
       </c>
       <c r="U749" s="10">
         <f>(O749/60+N749)-(L749/60+K749)</f>
@@ -64189,9 +64272,11 @@
       <c r="V749" s="10"/>
       <c r="W749" s="11">
         <f>T749+U749-Q749*0.5+V749</f>
-        <v>0</v>
-      </c>
-      <c r="X749" s="10"/>
+        <v>10.816666666666666</v>
+      </c>
+      <c r="X749" s="10">
+        <v>8</v>
+      </c>
       <c r="Y749" t="s">
         <v>11</v>
       </c>
@@ -64218,9 +64303,21 @@
         <v>5</v>
       </c>
       <c r="D750" s="1"/>
+      <c r="E750">
+        <v>10</v>
+      </c>
+      <c r="F750">
+        <v>48</v>
+      </c>
       <c r="G750" s="79" t="s">
         <v>6</v>
       </c>
+      <c r="H750">
+        <v>17</v>
+      </c>
+      <c r="I750">
+        <v>30</v>
+      </c>
       <c r="J750" s="82" t="s">
         <v>17</v>
       </c>
@@ -64228,12 +64325,14 @@
         <v>6</v>
       </c>
       <c r="P750" s="1"/>
-      <c r="Q750" s="3"/>
+      <c r="Q750" s="3">
+        <v>1</v>
+      </c>
       <c r="R750" s="5"/>
       <c r="S750" s="4"/>
       <c r="T750" s="10">
         <f>(I750/60+H750)-(F750/60+E750)</f>
-        <v>0</v>
+        <v>6.6999999999999993</v>
       </c>
       <c r="U750" s="10">
         <f>(O750/60+N750)-(L750/60+K750)</f>
@@ -64242,28 +64341,30 @@
       <c r="V750" s="10"/>
       <c r="W750" s="11">
         <f>T750+U750-Q750*0.5+V750</f>
-        <v>0</v>
-      </c>
-      <c r="X750" s="10"/>
+        <v>6.1999999999999993</v>
+      </c>
+      <c r="X750" s="10">
+        <v>8</v>
+      </c>
       <c r="Y750" s="12">
         <f>SUM(W746:W750)</f>
-        <v>0</v>
+        <v>37.766666666666666</v>
       </c>
       <c r="Z750" s="10">
         <f>Y750-(8*(5-Z748))+SUM(S746:S750)*8</f>
-        <v>-40</v>
+        <v>-2.2333333333333343</v>
       </c>
       <c r="AA750" s="10">
         <f>AA743+Z750</f>
-        <v>-151.69999999999999</v>
+        <v>-73.933333333333337</v>
       </c>
       <c r="AB750" s="10">
         <f>AB743+Z750</f>
-        <v>-148.05333333333334</v>
+        <v>-70.28666666666669</v>
       </c>
       <c r="AC750" s="10">
         <f>AC743+Y750</f>
-        <v>406.8</v>
+        <v>444.56666666666666</v>
       </c>
     </row>
     <row r="751" spans="1:33" x14ac:dyDescent="0.25">
@@ -64303,14 +64404,16 @@
       <c r="X751" s="68"/>
       <c r="Y751" s="120">
         <f>SUM(X746:X750)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="Z751" s="66"/>
       <c r="AA751" s="66"/>
-      <c r="AB751" s="69"/>
+      <c r="AB751" s="69" t="s">
+        <v>285</v>
+      </c>
       <c r="AC751" s="129">
         <f>AC744+Y751</f>
-        <v>406.5</v>
+        <v>444.5</v>
       </c>
       <c r="AD751" s="124"/>
       <c r="AE751" s="58"/>
@@ -64322,7 +64425,7 @@
         <v>43779</v>
       </c>
       <c r="B752" s="6" t="s">
-        <v>298</v>
+        <v>26</v>
       </c>
       <c r="C752" s="1"/>
       <c r="D752" s="1"/>
@@ -64376,9 +64479,21 @@
         <v>1</v>
       </c>
       <c r="D753" s="1"/>
+      <c r="E753">
+        <v>8</v>
+      </c>
+      <c r="F753">
+        <v>50</v>
+      </c>
       <c r="G753" s="79" t="s">
         <v>6</v>
       </c>
+      <c r="H753">
+        <v>17</v>
+      </c>
+      <c r="I753">
+        <v>5</v>
+      </c>
       <c r="J753" s="82" t="s">
         <v>17</v>
       </c>
@@ -64386,12 +64501,14 @@
         <v>6</v>
       </c>
       <c r="P753" s="1"/>
-      <c r="Q753" s="3"/>
+      <c r="Q753" s="3">
+        <v>1</v>
+      </c>
       <c r="R753" s="5"/>
       <c r="S753" s="4"/>
       <c r="T753" s="10">
         <f>(I753/60+H753)-(F753/60+E753)</f>
-        <v>0</v>
+        <v>8.2499999999999982</v>
       </c>
       <c r="U753" s="10">
         <f>(O753/60+N753)-(L753/60+K753)</f>
@@ -64400,7 +64517,7 @@
       <c r="V753" s="10"/>
       <c r="W753" s="11">
         <f>T753+U753-Q753*0.5+V753</f>
-        <v>0</v>
+        <v>7.7499999999999982</v>
       </c>
       <c r="X753" s="106"/>
       <c r="AC753" s="8"/>
@@ -64414,8 +64531,20 @@
         <v>2</v>
       </c>
       <c r="D754" s="1"/>
+      <c r="E754">
+        <v>8</v>
+      </c>
+      <c r="F754">
+        <v>23</v>
+      </c>
       <c r="G754" s="79" t="s">
         <v>6</v>
+      </c>
+      <c r="H754">
+        <v>17</v>
+      </c>
+      <c r="I754">
+        <v>5</v>
       </c>
       <c r="J754" s="82" t="s">
         <v>17</v>
@@ -64429,7 +64558,7 @@
       <c r="S754" s="4"/>
       <c r="T754" s="10">
         <f>(I754/60+H754)-(F754/60+E754)</f>
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="U754" s="10">
         <f>(O754/60+N754)-(L754/60+K754)</f>
@@ -64438,7 +64567,7 @@
       <c r="V754" s="10"/>
       <c r="W754" s="11">
         <f>T754+U754-Q754*0.5+V754</f>
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="X754" s="10"/>
       <c r="Z754" t="s">
@@ -64454,8 +64583,20 @@
         <v>3</v>
       </c>
       <c r="D755" s="1"/>
+      <c r="E755">
+        <v>8</v>
+      </c>
+      <c r="F755">
+        <v>21</v>
+      </c>
       <c r="G755" s="79" t="s">
         <v>6</v>
+      </c>
+      <c r="H755">
+        <v>16</v>
+      </c>
+      <c r="I755">
+        <v>0</v>
       </c>
       <c r="J755" s="82" t="s">
         <v>17</v>
@@ -64469,7 +64610,7 @@
       <c r="S755" s="4"/>
       <c r="T755" s="10">
         <f>(I755/60+H755)-(F755/60+E755)</f>
-        <v>0</v>
+        <v>7.65</v>
       </c>
       <c r="U755" s="10">
         <f>(O755/60+N755)-(L755/60+K755)</f>
@@ -64478,7 +64619,7 @@
       <c r="V755" s="10"/>
       <c r="W755" s="11">
         <f>T755+U755-Q755*0.5+V755</f>
-        <v>0</v>
+        <v>7.65</v>
       </c>
       <c r="X755" s="10"/>
       <c r="Z755" s="74">
@@ -64576,23 +64717,23 @@
       <c r="X757" s="10"/>
       <c r="Y757" s="12">
         <f>SUM(W753:W757)</f>
-        <v>0</v>
+        <v>24.099999999999994</v>
       </c>
       <c r="Z757" s="10">
         <f>Y757-(8*(5-Z755))+SUM(S753:S757)*8</f>
-        <v>-40</v>
+        <v>-15.900000000000006</v>
       </c>
       <c r="AA757" s="10">
         <f>AA750+Z757</f>
-        <v>-191.7</v>
+        <v>-89.833333333333343</v>
       </c>
       <c r="AB757" s="10">
         <f>AB750+Z757</f>
-        <v>-188.05333333333334</v>
+        <v>-86.186666666666696</v>
       </c>
       <c r="AC757" s="10">
         <f>AC750+Y757</f>
-        <v>406.8</v>
+        <v>468.66666666666663</v>
       </c>
     </row>
     <row r="758" spans="1:33" x14ac:dyDescent="0.25">
@@ -64636,10 +64777,12 @@
       </c>
       <c r="Z758" s="66"/>
       <c r="AA758" s="66"/>
-      <c r="AB758" s="69"/>
+      <c r="AB758" s="69" t="s">
+        <v>285</v>
+      </c>
       <c r="AC758" s="129">
         <f>AC751+Y758</f>
-        <v>406.5</v>
+        <v>444.5</v>
       </c>
       <c r="AD758" s="124"/>
       <c r="AE758" s="58"/>
@@ -64913,15 +65056,15 @@
       </c>
       <c r="AA764" s="10">
         <f>AA757+Z764</f>
-        <v>-231.7</v>
+        <v>-129.83333333333334</v>
       </c>
       <c r="AB764" s="10">
         <f>AB757+Z764</f>
-        <v>-228.05333333333334</v>
+        <v>-126.1866666666667</v>
       </c>
       <c r="AC764" s="10">
         <f>AC757+Y764</f>
-        <v>406.8</v>
+        <v>468.66666666666663</v>
       </c>
     </row>
     <row r="765" spans="1:33" x14ac:dyDescent="0.25">
@@ -64968,7 +65111,7 @@
       <c r="AB765" s="69"/>
       <c r="AC765" s="129">
         <f>AC758+Y765</f>
-        <v>406.5</v>
+        <v>444.5</v>
       </c>
       <c r="AD765" s="124"/>
       <c r="AE765" s="58"/>
@@ -65242,15 +65385,15 @@
       </c>
       <c r="AA771" s="10">
         <f>AA764+Z771</f>
-        <v>-271.7</v>
+        <v>-169.83333333333334</v>
       </c>
       <c r="AB771" s="10">
         <f>AB764+Z771</f>
-        <v>-268.05333333333334</v>
+        <v>-166.1866666666667</v>
       </c>
       <c r="AC771" s="10">
         <f>AC764+Y771</f>
-        <v>406.8</v>
+        <v>468.66666666666663</v>
       </c>
     </row>
     <row r="772" spans="1:33" x14ac:dyDescent="0.25">
@@ -65297,7 +65440,7 @@
       <c r="AB772" s="69"/>
       <c r="AC772" s="129">
         <f>AC765+Y772</f>
-        <v>406.5</v>
+        <v>444.5</v>
       </c>
       <c r="AD772" s="124"/>
       <c r="AE772" s="58"/>
@@ -65571,15 +65714,15 @@
       </c>
       <c r="AA778" s="10">
         <f>AA771+Z778</f>
-        <v>-311.7</v>
+        <v>-209.83333333333334</v>
       </c>
       <c r="AB778" s="10">
         <f>AB771+Z778</f>
-        <v>-308.05333333333334</v>
+        <v>-206.1866666666667</v>
       </c>
       <c r="AC778" s="10">
         <f>AC771+Y778</f>
-        <v>406.8</v>
+        <v>468.66666666666663</v>
       </c>
     </row>
     <row r="779" spans="1:33" x14ac:dyDescent="0.25">
@@ -65626,7 +65769,7 @@
       <c r="AB779" s="69"/>
       <c r="AC779" s="129">
         <f>AC772+Y779</f>
-        <v>406.5</v>
+        <v>444.5</v>
       </c>
       <c r="AD779" s="124"/>
       <c r="AE779" s="58"/>
@@ -65900,15 +66043,15 @@
       </c>
       <c r="AA785" s="10">
         <f>AA778+Z785</f>
-        <v>-351.7</v>
+        <v>-249.83333333333334</v>
       </c>
       <c r="AB785" s="10">
         <f>AB778+Z785</f>
-        <v>-348.05333333333334</v>
+        <v>-246.1866666666667</v>
       </c>
       <c r="AC785" s="10">
         <f>AC778+Y785</f>
-        <v>406.8</v>
+        <v>468.66666666666663</v>
       </c>
     </row>
     <row r="786" spans="1:33" x14ac:dyDescent="0.25">
@@ -65955,7 +66098,7 @@
       <c r="AB786" s="69"/>
       <c r="AC786" s="129">
         <f>AC779+Y786</f>
-        <v>406.5</v>
+        <v>444.5</v>
       </c>
       <c r="AD786" s="124"/>
       <c r="AE786" s="58"/>
@@ -66024,6 +66167,176 @@
     <mergeCell ref="K423:O423"/>
   </mergeCells>
   <conditionalFormatting sqref="Y216">
+    <cfRule type="colorScale" priority="111">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y209 Y307 Y300 Y293 Y286 Y279 Y272 Y265 Y258 Y251 Y244 Y237 Y230 Y223 Y172 Y178 Y184 Y190 Y196 Y202">
+    <cfRule type="colorScale" priority="110">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD273">
+    <cfRule type="colorScale" priority="108">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD218 AD309 AD225 AD232 AD239 AD246 AD253 AD260 AD266 AD281 AD288 AD295 AD302">
+    <cfRule type="colorScale" priority="107">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD211">
+    <cfRule type="colorScale" priority="106">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD204">
+    <cfRule type="colorScale" priority="105">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y314">
+    <cfRule type="colorScale" priority="104">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD316">
+    <cfRule type="colorScale" priority="103">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y321">
+    <cfRule type="colorScale" priority="102">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD323">
+    <cfRule type="colorScale" priority="101">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y328">
+    <cfRule type="colorScale" priority="100">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD330">
+    <cfRule type="colorScale" priority="99">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y335">
+    <cfRule type="colorScale" priority="98">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH333">
+    <cfRule type="colorScale" priority="97">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y342">
+    <cfRule type="colorScale" priority="96">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y349">
+    <cfRule type="colorScale" priority="94">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y356">
+    <cfRule type="colorScale" priority="92">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y363">
     <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66033,8 +66346,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y209 Y307 Y300 Y293 Y286 Y279 Y272 Y265 Y258 Y251 Y244 Y237 Y230 Y223 Y172 Y178 Y184 Y190 Y196 Y202">
-    <cfRule type="colorScale" priority="89">
+  <conditionalFormatting sqref="Y370">
+    <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
@@ -66043,48 +66356,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD273">
-    <cfRule type="colorScale" priority="87">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD218 AD309 AD225 AD232 AD239 AD246 AD253 AD260 AD266 AD281 AD288 AD295 AD302">
+  <conditionalFormatting sqref="Y377">
     <cfRule type="colorScale" priority="86">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD211">
-    <cfRule type="colorScale" priority="85">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD204">
-    <cfRule type="colorScale" priority="84">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y314">
-    <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
@@ -66093,17 +66366,27 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD316">
+  <conditionalFormatting sqref="Z384">
+    <cfRule type="colorScale" priority="84">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z391">
     <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
         <color theme="0"/>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y321">
+  <conditionalFormatting sqref="Z398">
     <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66113,17 +66396,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD323">
+  <conditionalFormatting sqref="Z405">
     <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
         <color theme="0"/>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y328">
+  <conditionalFormatting sqref="Z412">
     <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66133,17 +66416,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD330">
+  <conditionalFormatting sqref="Z419">
     <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
         <color theme="0"/>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y335">
+  <conditionalFormatting sqref="Z426">
     <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66153,17 +66436,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AH333">
+  <conditionalFormatting sqref="Z433">
     <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
         <color theme="0"/>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y342">
+  <conditionalFormatting sqref="Z440">
     <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66173,7 +66456,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y349">
+  <conditionalFormatting sqref="Z447">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z454">
     <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66183,7 +66476,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y356">
+  <conditionalFormatting sqref="Z461">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z468">
     <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66193,7 +66496,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y363">
+  <conditionalFormatting sqref="Z475">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z482">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66203,7 +66516,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y370">
+  <conditionalFormatting sqref="Z489">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z496">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66213,7 +66536,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y377">
+  <conditionalFormatting sqref="Z503">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z510">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66223,7 +66556,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z384">
+  <conditionalFormatting sqref="Z517">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z524">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66233,7 +66576,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z391">
+  <conditionalFormatting sqref="Z531">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="5"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z538">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66243,7 +66596,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z398">
+  <conditionalFormatting sqref="Z545">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66253,7 +66606,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z405">
+  <conditionalFormatting sqref="Z552">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66263,7 +66616,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z412">
+  <conditionalFormatting sqref="Z559">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66273,7 +66626,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z419">
+  <conditionalFormatting sqref="Z566">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66283,7 +66636,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z426">
+  <conditionalFormatting sqref="Z573">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66293,7 +66646,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z433">
+  <conditionalFormatting sqref="Z580">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66303,7 +66656,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z440">
+  <conditionalFormatting sqref="Z587">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66313,7 +66666,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z447">
+  <conditionalFormatting sqref="Z594">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66323,7 +66676,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z454">
+  <conditionalFormatting sqref="Z601">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66333,7 +66686,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z461">
+  <conditionalFormatting sqref="Z608">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66343,7 +66696,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z468">
+  <conditionalFormatting sqref="Z615">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66353,7 +66706,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z475">
+  <conditionalFormatting sqref="Z622">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66363,7 +66716,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z482">
+  <conditionalFormatting sqref="Z629">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66373,7 +66726,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z489">
+  <conditionalFormatting sqref="Z636">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66383,7 +66736,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z496">
+  <conditionalFormatting sqref="Z643">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66393,7 +66746,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z503">
+  <conditionalFormatting sqref="Z650">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66403,7 +66756,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z510">
+  <conditionalFormatting sqref="Z657">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66413,7 +66766,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z517">
+  <conditionalFormatting sqref="Z664">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66423,7 +66776,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z524">
+  <conditionalFormatting sqref="Z671">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66433,7 +66786,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z531">
+  <conditionalFormatting sqref="Z678">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66443,7 +66796,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z538">
+  <conditionalFormatting sqref="Z685">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66453,7 +66806,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z545">
+  <conditionalFormatting sqref="Z692">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66463,7 +66816,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z552">
+  <conditionalFormatting sqref="Z699">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66473,7 +66826,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z559">
+  <conditionalFormatting sqref="Z706">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66483,7 +66836,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z566">
+  <conditionalFormatting sqref="Z713">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66493,7 +66846,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z573">
+  <conditionalFormatting sqref="Z720">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66503,47 +66856,47 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z580">
+  <conditionalFormatting sqref="AI544">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
         <color theme="0"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z587">
+  <conditionalFormatting sqref="AI537">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
         <color theme="0"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z594">
+  <conditionalFormatting sqref="AI530">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
         <color theme="0"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z601">
+  <conditionalFormatting sqref="AI523">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="5"/>
         <color theme="0"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z608">
+  <conditionalFormatting sqref="Z727">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66553,7 +66906,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z615">
+  <conditionalFormatting sqref="Z734">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66563,7 +66916,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z622">
+  <conditionalFormatting sqref="Z741">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66573,7 +66926,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z629">
+  <conditionalFormatting sqref="Z748">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66583,7 +66936,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z636">
+  <conditionalFormatting sqref="Z755">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66593,7 +66946,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z643">
+  <conditionalFormatting sqref="Z762">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66603,7 +66956,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z650">
+  <conditionalFormatting sqref="Z769">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66613,7 +66966,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z657">
+  <conditionalFormatting sqref="Z776">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66623,7 +66976,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z664">
+  <conditionalFormatting sqref="Z783">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -66633,218 +66986,394 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z671">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="W746:W750">
+    <cfRule type="dataBar" priority="21">
+      <dataBar>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{13AA8F12-1B0B-442E-936B-C6BABAD5B0D4}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z678">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="W739:W743">
+    <cfRule type="dataBar" priority="20">
+      <dataBar>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9B2E079C-EA53-43A6-9990-E9B2E01B2771}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z685">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="W732:W736">
+    <cfRule type="dataBar" priority="19">
+      <dataBar>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{484519BD-CFCE-4606-8EDE-2A5E60FE2802}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z692">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="W725:W729">
+    <cfRule type="dataBar" priority="18">
+      <dataBar>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B1192BE6-F5FE-40D5-9F0A-8D4649E208BD}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z699">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="W718:W722">
+    <cfRule type="dataBar" priority="17">
+      <dataBar>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{24C91A6A-01D0-44E9-BFCB-6F6F3C700ED4}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z706">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="W753:W757">
+    <cfRule type="dataBar" priority="16">
+      <dataBar>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{ACEB0313-5933-415E-A307-56526568FC4E}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z713">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="W760:W764">
+    <cfRule type="dataBar" priority="15">
+      <dataBar>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DB3157D5-9295-4532-A099-124301782E95}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z720">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="W767:W771">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0895FF1E-2D92-4441-8438-12DFC8350B32}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI544">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
+  <conditionalFormatting sqref="W774:W778">
+    <cfRule type="dataBar" priority="13">
+      <dataBar>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F4A0677C-93AF-49C5-9D78-35D6DF6520E9}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI537">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
+  <conditionalFormatting sqref="W781:W785">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D36858F4-ABB6-46F3-A3D1-BF300E30075F}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI530">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
+  <conditionalFormatting sqref="X746:X750">
+    <cfRule type="iconSet" priority="11">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI523">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
+  <conditionalFormatting sqref="X732:X736">
+    <cfRule type="iconSet" priority="10">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z727">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="X718:X722">
+    <cfRule type="iconSet" priority="9">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z734">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="X725:X729">
+    <cfRule type="iconSet" priority="8">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z741">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="X739:X743">
+    <cfRule type="iconSet" priority="7">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z748">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="X753:X757">
+    <cfRule type="iconSet" priority="6">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z755">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="X760:X764">
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z762">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="X767:X771">
+    <cfRule type="iconSet" priority="4">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z769">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="X774:X778">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z776">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z783">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="5"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
+  <conditionalFormatting sqref="X781:X785">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="7"/>
+        <cfvo type="num" val="8"/>
+      </iconSet>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{13AA8F12-1B0B-442E-936B-C6BABAD5B0D4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>8</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W746:W750</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9B2E079C-EA53-43A6-9990-E9B2E01B2771}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>8</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W739:W743</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{484519BD-CFCE-4606-8EDE-2A5E60FE2802}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>8</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W732:W736</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B1192BE6-F5FE-40D5-9F0A-8D4649E208BD}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>8</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W725:W729</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{24C91A6A-01D0-44E9-BFCB-6F6F3C700ED4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>8</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W718:W722</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{ACEB0313-5933-415E-A307-56526568FC4E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>8</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W753:W757</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{DB3157D5-9295-4532-A099-124301782E95}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>8</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W760:W764</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0895FF1E-2D92-4441-8438-12DFC8350B32}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>8</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W767:W771</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F4A0677C-93AF-49C5-9D78-35D6DF6520E9}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>8</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W774:W778</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D36858F4-ABB6-46F3-A3D1-BF300E30075F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>8</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>W781:W785</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated the time report to week 31 of 2020
</commit_message>
<xml_diff>
--- a/tidsrapport/tidsrapportering3.xlsx
+++ b/tidsrapport/tidsrapportering3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehaagse\Desktop\code_snippets\tidsrapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A254034-78D8-4E16-8CB1-F78F8DC0A761}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FF2F83-A056-4636-B89C-BAD8EE6EF791}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1719,6 +1721,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1728,9 +1733,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10355,20 +10357,20 @@
       <c r="A4" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="139" t="s">
+      <c r="C4" s="142" t="s">
         <v>160</v>
       </c>
-      <c r="D4" s="139"/>
-      <c r="E4" s="139"/>
-      <c r="F4" s="139"/>
-      <c r="G4" s="139"/>
-      <c r="I4" s="139" t="s">
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="I4" s="142" t="s">
         <v>161</v>
       </c>
-      <c r="J4" s="139"/>
-      <c r="K4" s="139"/>
-      <c r="L4" s="139"/>
-      <c r="M4" s="139"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="142"/>
       <c r="N4" s="31"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="40" t="s">
@@ -23533,21 +23535,21 @@
       </c>
       <c r="C2" s="86"/>
       <c r="D2" s="86"/>
-      <c r="E2" s="141" t="s">
+      <c r="E2" s="144" t="s">
         <v>251</v>
       </c>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
       <c r="J2" s="87"/>
-      <c r="K2" s="141" t="s">
+      <c r="K2" s="144" t="s">
         <v>252</v>
       </c>
-      <c r="L2" s="141"/>
-      <c r="M2" s="141"/>
-      <c r="N2" s="141"/>
-      <c r="O2" s="141"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="144"/>
+      <c r="O2" s="144"/>
       <c r="P2" s="86"/>
       <c r="Q2" s="94" t="s">
         <v>18</v>
@@ -37167,21 +37169,21 @@
       </c>
       <c r="C262" s="1"/>
       <c r="D262" s="1"/>
-      <c r="E262" s="140" t="s">
+      <c r="E262" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F262" s="140"/>
-      <c r="G262" s="140"/>
-      <c r="H262" s="140"/>
-      <c r="I262" s="140"/>
+      <c r="F262" s="143"/>
+      <c r="G262" s="143"/>
+      <c r="H262" s="143"/>
+      <c r="I262" s="143"/>
       <c r="J262" s="42"/>
-      <c r="K262" s="140" t="s">
+      <c r="K262" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L262" s="140"/>
-      <c r="M262" s="140"/>
-      <c r="N262" s="140"/>
-      <c r="O262" s="140"/>
+      <c r="L262" s="143"/>
+      <c r="M262" s="143"/>
+      <c r="N262" s="143"/>
+      <c r="O262" s="143"/>
       <c r="P262" s="1"/>
       <c r="Q262" s="93" t="s">
         <v>18</v>
@@ -37595,21 +37597,21 @@
       </c>
       <c r="C269" s="1"/>
       <c r="D269" s="1"/>
-      <c r="E269" s="140" t="s">
+      <c r="E269" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F269" s="140"/>
-      <c r="G269" s="140"/>
-      <c r="H269" s="140"/>
-      <c r="I269" s="140"/>
+      <c r="F269" s="143"/>
+      <c r="G269" s="143"/>
+      <c r="H269" s="143"/>
+      <c r="I269" s="143"/>
       <c r="J269" s="42"/>
-      <c r="K269" s="140" t="s">
+      <c r="K269" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L269" s="140"/>
-      <c r="M269" s="140"/>
-      <c r="N269" s="140"/>
-      <c r="O269" s="140"/>
+      <c r="L269" s="143"/>
+      <c r="M269" s="143"/>
+      <c r="N269" s="143"/>
+      <c r="O269" s="143"/>
       <c r="P269" s="1"/>
       <c r="Q269" s="93" t="s">
         <v>18</v>
@@ -38008,21 +38010,21 @@
       </c>
       <c r="C276" s="1"/>
       <c r="D276" s="1"/>
-      <c r="E276" s="140" t="s">
+      <c r="E276" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F276" s="140"/>
-      <c r="G276" s="140"/>
-      <c r="H276" s="140"/>
-      <c r="I276" s="140"/>
+      <c r="F276" s="143"/>
+      <c r="G276" s="143"/>
+      <c r="H276" s="143"/>
+      <c r="I276" s="143"/>
       <c r="J276" s="42"/>
-      <c r="K276" s="140" t="s">
+      <c r="K276" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L276" s="140"/>
-      <c r="M276" s="140"/>
-      <c r="N276" s="140"/>
-      <c r="O276" s="140"/>
+      <c r="L276" s="143"/>
+      <c r="M276" s="143"/>
+      <c r="N276" s="143"/>
+      <c r="O276" s="143"/>
       <c r="P276" s="1"/>
       <c r="Q276" s="93" t="s">
         <v>18</v>
@@ -38400,21 +38402,21 @@
       </c>
       <c r="C283" s="1"/>
       <c r="D283" s="1"/>
-      <c r="E283" s="140" t="s">
+      <c r="E283" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F283" s="140"/>
-      <c r="G283" s="140"/>
-      <c r="H283" s="140"/>
-      <c r="I283" s="140"/>
+      <c r="F283" s="143"/>
+      <c r="G283" s="143"/>
+      <c r="H283" s="143"/>
+      <c r="I283" s="143"/>
       <c r="J283" s="42"/>
-      <c r="K283" s="140" t="s">
+      <c r="K283" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L283" s="140"/>
-      <c r="M283" s="140"/>
-      <c r="N283" s="140"/>
-      <c r="O283" s="140"/>
+      <c r="L283" s="143"/>
+      <c r="M283" s="143"/>
+      <c r="N283" s="143"/>
+      <c r="O283" s="143"/>
       <c r="P283" s="1"/>
       <c r="Q283" s="93" t="s">
         <v>18</v>
@@ -38756,21 +38758,21 @@
       </c>
       <c r="C290" s="1"/>
       <c r="D290" s="1"/>
-      <c r="E290" s="140" t="s">
+      <c r="E290" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F290" s="140"/>
-      <c r="G290" s="140"/>
-      <c r="H290" s="140"/>
-      <c r="I290" s="140"/>
+      <c r="F290" s="143"/>
+      <c r="G290" s="143"/>
+      <c r="H290" s="143"/>
+      <c r="I290" s="143"/>
       <c r="J290" s="42"/>
-      <c r="K290" s="140" t="s">
+      <c r="K290" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L290" s="140"/>
-      <c r="M290" s="140"/>
-      <c r="N290" s="140"/>
-      <c r="O290" s="140"/>
+      <c r="L290" s="143"/>
+      <c r="M290" s="143"/>
+      <c r="N290" s="143"/>
+      <c r="O290" s="143"/>
       <c r="P290" s="1"/>
       <c r="Q290" s="93" t="s">
         <v>18</v>
@@ -39119,21 +39121,21 @@
       </c>
       <c r="C297" s="1"/>
       <c r="D297" s="1"/>
-      <c r="E297" s="140" t="s">
+      <c r="E297" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F297" s="140"/>
-      <c r="G297" s="140"/>
-      <c r="H297" s="140"/>
-      <c r="I297" s="140"/>
+      <c r="F297" s="143"/>
+      <c r="G297" s="143"/>
+      <c r="H297" s="143"/>
+      <c r="I297" s="143"/>
       <c r="J297" s="42"/>
-      <c r="K297" s="140" t="s">
+      <c r="K297" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L297" s="140"/>
-      <c r="M297" s="140"/>
-      <c r="N297" s="140"/>
-      <c r="O297" s="140"/>
+      <c r="L297" s="143"/>
+      <c r="M297" s="143"/>
+      <c r="N297" s="143"/>
+      <c r="O297" s="143"/>
       <c r="P297" s="1"/>
       <c r="Q297" s="93" t="s">
         <v>18</v>
@@ -39538,21 +39540,21 @@
       </c>
       <c r="C304" s="1"/>
       <c r="D304" s="1"/>
-      <c r="E304" s="140" t="s">
+      <c r="E304" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F304" s="140"/>
-      <c r="G304" s="140"/>
-      <c r="H304" s="140"/>
-      <c r="I304" s="140"/>
+      <c r="F304" s="143"/>
+      <c r="G304" s="143"/>
+      <c r="H304" s="143"/>
+      <c r="I304" s="143"/>
       <c r="J304" s="42"/>
-      <c r="K304" s="140" t="s">
+      <c r="K304" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L304" s="140"/>
-      <c r="M304" s="140"/>
-      <c r="N304" s="140"/>
-      <c r="O304" s="140"/>
+      <c r="L304" s="143"/>
+      <c r="M304" s="143"/>
+      <c r="N304" s="143"/>
+      <c r="O304" s="143"/>
       <c r="P304" s="1"/>
       <c r="Q304" s="93" t="s">
         <v>18</v>
@@ -39947,21 +39949,21 @@
       </c>
       <c r="C311" s="1"/>
       <c r="D311" s="1"/>
-      <c r="E311" s="140" t="s">
+      <c r="E311" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F311" s="140"/>
-      <c r="G311" s="140"/>
-      <c r="H311" s="140"/>
-      <c r="I311" s="140"/>
+      <c r="F311" s="143"/>
+      <c r="G311" s="143"/>
+      <c r="H311" s="143"/>
+      <c r="I311" s="143"/>
       <c r="J311" s="42"/>
-      <c r="K311" s="140" t="s">
+      <c r="K311" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L311" s="140"/>
-      <c r="M311" s="140"/>
-      <c r="N311" s="140"/>
-      <c r="O311" s="140"/>
+      <c r="L311" s="143"/>
+      <c r="M311" s="143"/>
+      <c r="N311" s="143"/>
+      <c r="O311" s="143"/>
       <c r="P311" s="1"/>
       <c r="Q311" s="93" t="s">
         <v>18</v>
@@ -40364,21 +40366,21 @@
       </c>
       <c r="C318" s="1"/>
       <c r="D318" s="1"/>
-      <c r="E318" s="140" t="s">
+      <c r="E318" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F318" s="140"/>
-      <c r="G318" s="140"/>
-      <c r="H318" s="140"/>
-      <c r="I318" s="140"/>
+      <c r="F318" s="143"/>
+      <c r="G318" s="143"/>
+      <c r="H318" s="143"/>
+      <c r="I318" s="143"/>
       <c r="J318" s="42"/>
-      <c r="K318" s="140" t="s">
+      <c r="K318" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L318" s="140"/>
-      <c r="M318" s="140"/>
-      <c r="N318" s="140"/>
-      <c r="O318" s="140"/>
+      <c r="L318" s="143"/>
+      <c r="M318" s="143"/>
+      <c r="N318" s="143"/>
+      <c r="O318" s="143"/>
       <c r="P318" s="1"/>
       <c r="Q318" s="93" t="s">
         <v>18</v>
@@ -40791,21 +40793,21 @@
       </c>
       <c r="C325" s="1"/>
       <c r="D325" s="1"/>
-      <c r="E325" s="140" t="s">
+      <c r="E325" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F325" s="140"/>
-      <c r="G325" s="140"/>
-      <c r="H325" s="140"/>
-      <c r="I325" s="140"/>
+      <c r="F325" s="143"/>
+      <c r="G325" s="143"/>
+      <c r="H325" s="143"/>
+      <c r="I325" s="143"/>
       <c r="J325" s="42"/>
-      <c r="K325" s="140" t="s">
+      <c r="K325" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L325" s="140"/>
-      <c r="M325" s="140"/>
-      <c r="N325" s="140"/>
-      <c r="O325" s="140"/>
+      <c r="L325" s="143"/>
+      <c r="M325" s="143"/>
+      <c r="N325" s="143"/>
+      <c r="O325" s="143"/>
       <c r="P325" s="1"/>
       <c r="Q325" s="93" t="s">
         <v>18</v>
@@ -41197,21 +41199,21 @@
       </c>
       <c r="C332" s="1"/>
       <c r="D332" s="1"/>
-      <c r="E332" s="140" t="s">
+      <c r="E332" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F332" s="140"/>
-      <c r="G332" s="140"/>
-      <c r="H332" s="140"/>
-      <c r="I332" s="140"/>
+      <c r="F332" s="143"/>
+      <c r="G332" s="143"/>
+      <c r="H332" s="143"/>
+      <c r="I332" s="143"/>
       <c r="J332" s="42"/>
-      <c r="K332" s="140" t="s">
+      <c r="K332" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L332" s="140"/>
-      <c r="M332" s="140"/>
-      <c r="N332" s="140"/>
-      <c r="O332" s="140"/>
+      <c r="L332" s="143"/>
+      <c r="M332" s="143"/>
+      <c r="N332" s="143"/>
+      <c r="O332" s="143"/>
       <c r="P332" s="1"/>
       <c r="Q332" s="93" t="s">
         <v>18</v>
@@ -41622,21 +41624,21 @@
       </c>
       <c r="C339" s="1"/>
       <c r="D339" s="1"/>
-      <c r="E339" s="140" t="s">
+      <c r="E339" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F339" s="140"/>
-      <c r="G339" s="140"/>
-      <c r="H339" s="140"/>
-      <c r="I339" s="140"/>
+      <c r="F339" s="143"/>
+      <c r="G339" s="143"/>
+      <c r="H339" s="143"/>
+      <c r="I339" s="143"/>
       <c r="J339" s="42"/>
-      <c r="K339" s="140" t="s">
+      <c r="K339" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L339" s="140"/>
-      <c r="M339" s="140"/>
-      <c r="N339" s="140"/>
-      <c r="O339" s="140"/>
+      <c r="L339" s="143"/>
+      <c r="M339" s="143"/>
+      <c r="N339" s="143"/>
+      <c r="O339" s="143"/>
       <c r="P339" s="1"/>
       <c r="Q339" s="93" t="s">
         <v>18</v>
@@ -42032,21 +42034,21 @@
       </c>
       <c r="C346" s="1"/>
       <c r="D346" s="1"/>
-      <c r="E346" s="140" t="s">
+      <c r="E346" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F346" s="140"/>
-      <c r="G346" s="140"/>
-      <c r="H346" s="140"/>
-      <c r="I346" s="140"/>
+      <c r="F346" s="143"/>
+      <c r="G346" s="143"/>
+      <c r="H346" s="143"/>
+      <c r="I346" s="143"/>
       <c r="J346" s="42"/>
-      <c r="K346" s="140" t="s">
+      <c r="K346" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L346" s="140"/>
-      <c r="M346" s="140"/>
-      <c r="N346" s="140"/>
-      <c r="O346" s="140"/>
+      <c r="L346" s="143"/>
+      <c r="M346" s="143"/>
+      <c r="N346" s="143"/>
+      <c r="O346" s="143"/>
       <c r="P346" s="1"/>
       <c r="Q346" s="93" t="s">
         <v>18</v>
@@ -42411,21 +42413,21 @@
       </c>
       <c r="C353" s="1"/>
       <c r="D353" s="1"/>
-      <c r="E353" s="140" t="s">
+      <c r="E353" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F353" s="140"/>
-      <c r="G353" s="140"/>
-      <c r="H353" s="140"/>
-      <c r="I353" s="140"/>
+      <c r="F353" s="143"/>
+      <c r="G353" s="143"/>
+      <c r="H353" s="143"/>
+      <c r="I353" s="143"/>
       <c r="J353" s="42"/>
-      <c r="K353" s="140" t="s">
+      <c r="K353" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L353" s="140"/>
-      <c r="M353" s="140"/>
-      <c r="N353" s="140"/>
-      <c r="O353" s="140"/>
+      <c r="L353" s="143"/>
+      <c r="M353" s="143"/>
+      <c r="N353" s="143"/>
+      <c r="O353" s="143"/>
       <c r="P353" s="1"/>
       <c r="Q353" s="93" t="s">
         <v>18</v>
@@ -42782,21 +42784,21 @@
       </c>
       <c r="C360" s="1"/>
       <c r="D360" s="1"/>
-      <c r="E360" s="140" t="s">
+      <c r="E360" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F360" s="140"/>
-      <c r="G360" s="140"/>
-      <c r="H360" s="140"/>
-      <c r="I360" s="140"/>
+      <c r="F360" s="143"/>
+      <c r="G360" s="143"/>
+      <c r="H360" s="143"/>
+      <c r="I360" s="143"/>
       <c r="J360" s="42"/>
-      <c r="K360" s="140" t="s">
+      <c r="K360" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L360" s="140"/>
-      <c r="M360" s="140"/>
-      <c r="N360" s="140"/>
-      <c r="O360" s="140"/>
+      <c r="L360" s="143"/>
+      <c r="M360" s="143"/>
+      <c r="N360" s="143"/>
+      <c r="O360" s="143"/>
       <c r="P360" s="1"/>
       <c r="Q360" s="93" t="s">
         <v>18</v>
@@ -43164,21 +43166,21 @@
       </c>
       <c r="C367" s="1"/>
       <c r="D367" s="1"/>
-      <c r="E367" s="140" t="s">
+      <c r="E367" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F367" s="140"/>
-      <c r="G367" s="140"/>
-      <c r="H367" s="140"/>
-      <c r="I367" s="140"/>
+      <c r="F367" s="143"/>
+      <c r="G367" s="143"/>
+      <c r="H367" s="143"/>
+      <c r="I367" s="143"/>
       <c r="J367" s="42"/>
-      <c r="K367" s="140" t="s">
+      <c r="K367" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L367" s="140"/>
-      <c r="M367" s="140"/>
-      <c r="N367" s="140"/>
-      <c r="O367" s="140"/>
+      <c r="L367" s="143"/>
+      <c r="M367" s="143"/>
+      <c r="N367" s="143"/>
+      <c r="O367" s="143"/>
       <c r="P367" s="1"/>
       <c r="Q367" s="93" t="s">
         <v>18</v>
@@ -43542,21 +43544,21 @@
       </c>
       <c r="C374" s="1"/>
       <c r="D374" s="1"/>
-      <c r="E374" s="140" t="s">
+      <c r="E374" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F374" s="140"/>
-      <c r="G374" s="140"/>
-      <c r="H374" s="140"/>
-      <c r="I374" s="140"/>
+      <c r="F374" s="143"/>
+      <c r="G374" s="143"/>
+      <c r="H374" s="143"/>
+      <c r="I374" s="143"/>
       <c r="J374" s="42"/>
-      <c r="K374" s="140" t="s">
+      <c r="K374" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L374" s="140"/>
-      <c r="M374" s="140"/>
-      <c r="N374" s="140"/>
-      <c r="O374" s="140"/>
+      <c r="L374" s="143"/>
+      <c r="M374" s="143"/>
+      <c r="N374" s="143"/>
+      <c r="O374" s="143"/>
       <c r="P374" s="1"/>
       <c r="Q374" s="93" t="s">
         <v>18</v>
@@ -43922,21 +43924,21 @@
       </c>
       <c r="C381" s="1"/>
       <c r="D381" s="1"/>
-      <c r="E381" s="140" t="s">
+      <c r="E381" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F381" s="140"/>
-      <c r="G381" s="140"/>
-      <c r="H381" s="140"/>
-      <c r="I381" s="140"/>
+      <c r="F381" s="143"/>
+      <c r="G381" s="143"/>
+      <c r="H381" s="143"/>
+      <c r="I381" s="143"/>
       <c r="J381" s="42"/>
-      <c r="K381" s="140" t="s">
+      <c r="K381" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L381" s="140"/>
-      <c r="M381" s="140"/>
-      <c r="N381" s="140"/>
-      <c r="O381" s="140"/>
+      <c r="L381" s="143"/>
+      <c r="M381" s="143"/>
+      <c r="N381" s="143"/>
+      <c r="O381" s="143"/>
       <c r="P381" s="1"/>
       <c r="Q381" s="93" t="s">
         <v>18</v>
@@ -44315,21 +44317,21 @@
       </c>
       <c r="C388" s="1"/>
       <c r="D388" s="1"/>
-      <c r="E388" s="140" t="s">
+      <c r="E388" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F388" s="140"/>
-      <c r="G388" s="140"/>
-      <c r="H388" s="140"/>
-      <c r="I388" s="140"/>
+      <c r="F388" s="143"/>
+      <c r="G388" s="143"/>
+      <c r="H388" s="143"/>
+      <c r="I388" s="143"/>
       <c r="J388" s="42"/>
-      <c r="K388" s="140" t="s">
+      <c r="K388" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L388" s="140"/>
-      <c r="M388" s="140"/>
-      <c r="N388" s="140"/>
-      <c r="O388" s="140"/>
+      <c r="L388" s="143"/>
+      <c r="M388" s="143"/>
+      <c r="N388" s="143"/>
+      <c r="O388" s="143"/>
       <c r="P388" s="1"/>
       <c r="Q388" s="93" t="s">
         <v>18</v>
@@ -44715,21 +44717,21 @@
       </c>
       <c r="C395" s="1"/>
       <c r="D395" s="1"/>
-      <c r="E395" s="140" t="s">
+      <c r="E395" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F395" s="140"/>
-      <c r="G395" s="140"/>
-      <c r="H395" s="140"/>
-      <c r="I395" s="140"/>
+      <c r="F395" s="143"/>
+      <c r="G395" s="143"/>
+      <c r="H395" s="143"/>
+      <c r="I395" s="143"/>
       <c r="J395" s="42"/>
-      <c r="K395" s="140" t="s">
+      <c r="K395" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L395" s="140"/>
-      <c r="M395" s="140"/>
-      <c r="N395" s="140"/>
-      <c r="O395" s="140"/>
+      <c r="L395" s="143"/>
+      <c r="M395" s="143"/>
+      <c r="N395" s="143"/>
+      <c r="O395" s="143"/>
       <c r="P395" s="1"/>
       <c r="Q395" s="93" t="s">
         <v>18</v>
@@ -45120,21 +45122,21 @@
       </c>
       <c r="C402" s="1"/>
       <c r="D402" s="1"/>
-      <c r="E402" s="140" t="s">
+      <c r="E402" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F402" s="140"/>
-      <c r="G402" s="140"/>
-      <c r="H402" s="140"/>
-      <c r="I402" s="140"/>
+      <c r="F402" s="143"/>
+      <c r="G402" s="143"/>
+      <c r="H402" s="143"/>
+      <c r="I402" s="143"/>
       <c r="J402" s="42"/>
-      <c r="K402" s="140" t="s">
+      <c r="K402" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L402" s="140"/>
-      <c r="M402" s="140"/>
-      <c r="N402" s="140"/>
-      <c r="O402" s="140"/>
+      <c r="L402" s="143"/>
+      <c r="M402" s="143"/>
+      <c r="N402" s="143"/>
+      <c r="O402" s="143"/>
       <c r="P402" s="1"/>
       <c r="Q402" s="93" t="s">
         <v>18</v>
@@ -45513,21 +45515,21 @@
       </c>
       <c r="C409" s="1"/>
       <c r="D409" s="1"/>
-      <c r="E409" s="140" t="s">
+      <c r="E409" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F409" s="140"/>
-      <c r="G409" s="140"/>
-      <c r="H409" s="140"/>
-      <c r="I409" s="140"/>
+      <c r="F409" s="143"/>
+      <c r="G409" s="143"/>
+      <c r="H409" s="143"/>
+      <c r="I409" s="143"/>
       <c r="J409" s="42"/>
-      <c r="K409" s="140" t="s">
+      <c r="K409" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L409" s="140"/>
-      <c r="M409" s="140"/>
-      <c r="N409" s="140"/>
-      <c r="O409" s="140"/>
+      <c r="L409" s="143"/>
+      <c r="M409" s="143"/>
+      <c r="N409" s="143"/>
+      <c r="O409" s="143"/>
       <c r="P409" s="1"/>
       <c r="Q409" s="93" t="s">
         <v>18</v>
@@ -45916,21 +45918,21 @@
       </c>
       <c r="C416" s="1"/>
       <c r="D416" s="1"/>
-      <c r="E416" s="140" t="s">
+      <c r="E416" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F416" s="140"/>
-      <c r="G416" s="140"/>
-      <c r="H416" s="140"/>
-      <c r="I416" s="140"/>
+      <c r="F416" s="143"/>
+      <c r="G416" s="143"/>
+      <c r="H416" s="143"/>
+      <c r="I416" s="143"/>
       <c r="J416" s="42"/>
-      <c r="K416" s="140" t="s">
+      <c r="K416" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L416" s="140"/>
-      <c r="M416" s="140"/>
-      <c r="N416" s="140"/>
-      <c r="O416" s="140"/>
+      <c r="L416" s="143"/>
+      <c r="M416" s="143"/>
+      <c r="N416" s="143"/>
+      <c r="O416" s="143"/>
       <c r="P416" s="1"/>
       <c r="Q416" s="93" t="s">
         <v>18</v>
@@ -46317,21 +46319,21 @@
       </c>
       <c r="C423" s="1"/>
       <c r="D423" s="1"/>
-      <c r="E423" s="140" t="s">
+      <c r="E423" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F423" s="140"/>
-      <c r="G423" s="140"/>
-      <c r="H423" s="140"/>
-      <c r="I423" s="140"/>
+      <c r="F423" s="143"/>
+      <c r="G423" s="143"/>
+      <c r="H423" s="143"/>
+      <c r="I423" s="143"/>
       <c r="J423" s="42"/>
-      <c r="K423" s="140" t="s">
+      <c r="K423" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L423" s="140"/>
-      <c r="M423" s="140"/>
-      <c r="N423" s="140"/>
-      <c r="O423" s="140"/>
+      <c r="L423" s="143"/>
+      <c r="M423" s="143"/>
+      <c r="N423" s="143"/>
+      <c r="O423" s="143"/>
       <c r="P423" s="1"/>
       <c r="Q423" s="93" t="s">
         <v>18</v>
@@ -46768,21 +46770,21 @@
       </c>
       <c r="C430" s="1"/>
       <c r="D430" s="1"/>
-      <c r="E430" s="140" t="s">
+      <c r="E430" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F430" s="140"/>
-      <c r="G430" s="140"/>
-      <c r="H430" s="140"/>
-      <c r="I430" s="140"/>
+      <c r="F430" s="143"/>
+      <c r="G430" s="143"/>
+      <c r="H430" s="143"/>
+      <c r="I430" s="143"/>
       <c r="J430" s="42"/>
-      <c r="K430" s="140" t="s">
+      <c r="K430" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L430" s="140"/>
-      <c r="M430" s="140"/>
-      <c r="N430" s="140"/>
-      <c r="O430" s="140"/>
+      <c r="L430" s="143"/>
+      <c r="M430" s="143"/>
+      <c r="N430" s="143"/>
+      <c r="O430" s="143"/>
       <c r="P430" s="1"/>
       <c r="Q430" s="93" t="s">
         <v>18</v>
@@ -47169,21 +47171,21 @@
       </c>
       <c r="C437" s="1"/>
       <c r="D437" s="1"/>
-      <c r="E437" s="140" t="s">
+      <c r="E437" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F437" s="140"/>
-      <c r="G437" s="140"/>
-      <c r="H437" s="140"/>
-      <c r="I437" s="140"/>
+      <c r="F437" s="143"/>
+      <c r="G437" s="143"/>
+      <c r="H437" s="143"/>
+      <c r="I437" s="143"/>
       <c r="J437" s="42"/>
-      <c r="K437" s="140" t="s">
+      <c r="K437" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L437" s="140"/>
-      <c r="M437" s="140"/>
-      <c r="N437" s="140"/>
-      <c r="O437" s="140"/>
+      <c r="L437" s="143"/>
+      <c r="M437" s="143"/>
+      <c r="N437" s="143"/>
+      <c r="O437" s="143"/>
       <c r="P437" s="1"/>
       <c r="Q437" s="93" t="s">
         <v>18</v>
@@ -47502,21 +47504,21 @@
       </c>
       <c r="C444" s="1"/>
       <c r="D444" s="1"/>
-      <c r="E444" s="140" t="s">
+      <c r="E444" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F444" s="140"/>
-      <c r="G444" s="140"/>
-      <c r="H444" s="140"/>
-      <c r="I444" s="140"/>
+      <c r="F444" s="143"/>
+      <c r="G444" s="143"/>
+      <c r="H444" s="143"/>
+      <c r="I444" s="143"/>
       <c r="J444" s="42"/>
-      <c r="K444" s="140" t="s">
+      <c r="K444" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L444" s="140"/>
-      <c r="M444" s="140"/>
-      <c r="N444" s="140"/>
-      <c r="O444" s="140"/>
+      <c r="L444" s="143"/>
+      <c r="M444" s="143"/>
+      <c r="N444" s="143"/>
+      <c r="O444" s="143"/>
       <c r="P444" s="1"/>
       <c r="Q444" s="93" t="s">
         <v>18</v>
@@ -47875,21 +47877,21 @@
       </c>
       <c r="C451" s="1"/>
       <c r="D451" s="1"/>
-      <c r="E451" s="140" t="s">
+      <c r="E451" s="143" t="s">
         <v>251</v>
       </c>
-      <c r="F451" s="140"/>
-      <c r="G451" s="140"/>
-      <c r="H451" s="140"/>
-      <c r="I451" s="140"/>
+      <c r="F451" s="143"/>
+      <c r="G451" s="143"/>
+      <c r="H451" s="143"/>
+      <c r="I451" s="143"/>
       <c r="J451" s="42"/>
-      <c r="K451" s="140" t="s">
+      <c r="K451" s="143" t="s">
         <v>252</v>
       </c>
-      <c r="L451" s="140"/>
-      <c r="M451" s="140"/>
-      <c r="N451" s="140"/>
-      <c r="O451" s="140"/>
+      <c r="L451" s="143"/>
+      <c r="M451" s="143"/>
+      <c r="N451" s="143"/>
+      <c r="O451" s="143"/>
       <c r="P451" s="1"/>
       <c r="Q451" s="93" t="s">
         <v>18</v>
@@ -67365,48 +67367,6 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="E437:I437"/>
-    <mergeCell ref="K437:O437"/>
-    <mergeCell ref="E430:I430"/>
-    <mergeCell ref="K430:O430"/>
-    <mergeCell ref="E409:I409"/>
-    <mergeCell ref="K409:O409"/>
-    <mergeCell ref="E416:I416"/>
-    <mergeCell ref="K416:O416"/>
-    <mergeCell ref="E423:I423"/>
-    <mergeCell ref="K423:O423"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="E304:I304"/>
-    <mergeCell ref="K304:O304"/>
-    <mergeCell ref="E283:I283"/>
-    <mergeCell ref="K283:O283"/>
-    <mergeCell ref="E276:I276"/>
-    <mergeCell ref="K276:O276"/>
-    <mergeCell ref="E269:I269"/>
-    <mergeCell ref="K269:O269"/>
-    <mergeCell ref="E262:I262"/>
-    <mergeCell ref="K262:O262"/>
-    <mergeCell ref="E339:I339"/>
-    <mergeCell ref="K339:O339"/>
-    <mergeCell ref="E290:I290"/>
-    <mergeCell ref="K290:O290"/>
-    <mergeCell ref="E311:I311"/>
-    <mergeCell ref="K311:O311"/>
-    <mergeCell ref="E318:I318"/>
-    <mergeCell ref="K318:O318"/>
-    <mergeCell ref="E325:I325"/>
-    <mergeCell ref="K325:O325"/>
-    <mergeCell ref="E297:I297"/>
-    <mergeCell ref="K297:O297"/>
-    <mergeCell ref="E332:I332"/>
-    <mergeCell ref="K332:O332"/>
-    <mergeCell ref="E346:I346"/>
-    <mergeCell ref="K346:O346"/>
-    <mergeCell ref="E353:I353"/>
-    <mergeCell ref="K353:O353"/>
-    <mergeCell ref="E360:I360"/>
-    <mergeCell ref="K360:O360"/>
     <mergeCell ref="E444:I444"/>
     <mergeCell ref="K444:O444"/>
     <mergeCell ref="E451:I451"/>
@@ -67423,6 +67383,48 @@
     <mergeCell ref="K395:O395"/>
     <mergeCell ref="E402:I402"/>
     <mergeCell ref="K402:O402"/>
+    <mergeCell ref="E346:I346"/>
+    <mergeCell ref="K346:O346"/>
+    <mergeCell ref="E353:I353"/>
+    <mergeCell ref="K353:O353"/>
+    <mergeCell ref="E360:I360"/>
+    <mergeCell ref="K360:O360"/>
+    <mergeCell ref="E339:I339"/>
+    <mergeCell ref="K339:O339"/>
+    <mergeCell ref="E290:I290"/>
+    <mergeCell ref="K290:O290"/>
+    <mergeCell ref="E311:I311"/>
+    <mergeCell ref="K311:O311"/>
+    <mergeCell ref="E318:I318"/>
+    <mergeCell ref="K318:O318"/>
+    <mergeCell ref="E325:I325"/>
+    <mergeCell ref="K325:O325"/>
+    <mergeCell ref="E297:I297"/>
+    <mergeCell ref="K297:O297"/>
+    <mergeCell ref="E332:I332"/>
+    <mergeCell ref="K332:O332"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="E304:I304"/>
+    <mergeCell ref="K304:O304"/>
+    <mergeCell ref="E283:I283"/>
+    <mergeCell ref="K283:O283"/>
+    <mergeCell ref="E276:I276"/>
+    <mergeCell ref="K276:O276"/>
+    <mergeCell ref="E269:I269"/>
+    <mergeCell ref="K269:O269"/>
+    <mergeCell ref="E262:I262"/>
+    <mergeCell ref="K262:O262"/>
+    <mergeCell ref="E437:I437"/>
+    <mergeCell ref="K437:O437"/>
+    <mergeCell ref="E430:I430"/>
+    <mergeCell ref="K430:O430"/>
+    <mergeCell ref="E409:I409"/>
+    <mergeCell ref="K409:O409"/>
+    <mergeCell ref="E416:I416"/>
+    <mergeCell ref="K416:O416"/>
+    <mergeCell ref="E423:I423"/>
+    <mergeCell ref="K423:O423"/>
   </mergeCells>
   <conditionalFormatting sqref="Y216">
     <cfRule type="colorScale" priority="161">
@@ -67434,7 +67436,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y307 Y209 Y300 Y293 Y286 Y279 Y272 Y265 Y258 Y251 Y244 Y237 Y230 Y223 Y172 Y178 Y184 Y190 Y196 Y202">
+  <conditionalFormatting sqref="Y209 Y307 Y300 Y293 Y286 Y279 Y272 Y265 Y258 Y251 Y244 Y237 Y230 Y223 Y172 Y178 Y184 Y190 Y196 Y202">
     <cfRule type="colorScale" priority="160">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -67454,7 +67456,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD309 AD218 AD225 AD232 AD239 AD246 AD253 AD260 AD266 AD281 AD288 AD295 AD302">
+  <conditionalFormatting sqref="AD218 AD309 AD225 AD232 AD239 AD246 AD253 AD260 AD266 AD281 AD288 AD295 AD302">
     <cfRule type="colorScale" priority="157">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -69044,7 +69046,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C196" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AG211" sqref="AG211"/>
+      <selection pane="bottomRight" activeCell="AI206" sqref="AI206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69105,21 +69107,21 @@
       </c>
       <c r="C2" s="86"/>
       <c r="D2" s="86"/>
-      <c r="E2" s="141" t="s">
+      <c r="E2" s="144" t="s">
         <v>251</v>
       </c>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
-      <c r="I2" s="141"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
       <c r="J2" s="87"/>
-      <c r="K2" s="141" t="s">
+      <c r="K2" s="144" t="s">
         <v>252</v>
       </c>
-      <c r="L2" s="141"/>
-      <c r="M2" s="141"/>
-      <c r="N2" s="141"/>
-      <c r="O2" s="141"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="144"/>
+      <c r="O2" s="144"/>
       <c r="P2" s="86"/>
       <c r="Q2" s="94" t="s">
         <v>18</v>
@@ -81691,28 +81693,28 @@
       <c r="A226" s="52">
         <v>44047</v>
       </c>
-      <c r="B226" s="142"/>
+      <c r="B226" s="139"/>
       <c r="C226" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D226" s="1"/>
-      <c r="E226" s="143"/>
-      <c r="F226" s="143"/>
+      <c r="E226" s="140"/>
+      <c r="F226" s="140"/>
       <c r="G226" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="H226" s="143"/>
-      <c r="I226" s="143"/>
+      <c r="H226" s="140"/>
+      <c r="I226" s="140"/>
       <c r="J226" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="K226" s="143"/>
-      <c r="L226" s="143"/>
+      <c r="K226" s="140"/>
+      <c r="L226" s="140"/>
       <c r="M226" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="N226" s="143"/>
-      <c r="O226" s="143"/>
+      <c r="N226" s="140"/>
+      <c r="O226" s="140"/>
       <c r="P226" s="1"/>
       <c r="Q226" s="3"/>
       <c r="R226" s="5"/>
@@ -81730,7 +81732,7 @@
         <f t="shared" si="214"/>
         <v>0</v>
       </c>
-      <c r="X226" s="144"/>
+      <c r="X226" s="141"/>
       <c r="Y226"/>
       <c r="Z226" t="s">
         <v>258</v>
@@ -81763,28 +81765,28 @@
       <c r="A227" s="52">
         <v>44048</v>
       </c>
-      <c r="B227" s="142"/>
+      <c r="B227" s="139"/>
       <c r="C227" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D227" s="1"/>
-      <c r="E227" s="143"/>
-      <c r="F227" s="143"/>
+      <c r="E227" s="140"/>
+      <c r="F227" s="140"/>
       <c r="G227" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="H227" s="143"/>
-      <c r="I227" s="143"/>
+      <c r="H227" s="140"/>
+      <c r="I227" s="140"/>
       <c r="J227" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="K227" s="143"/>
-      <c r="L227" s="143"/>
+      <c r="K227" s="140"/>
+      <c r="L227" s="140"/>
       <c r="M227" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="N227" s="143"/>
-      <c r="O227" s="143"/>
+      <c r="N227" s="140"/>
+      <c r="O227" s="140"/>
       <c r="P227" s="1"/>
       <c r="Q227" s="3"/>
       <c r="R227" s="5"/>
@@ -81802,7 +81804,7 @@
         <f t="shared" si="214"/>
         <v>0</v>
       </c>
-      <c r="X227" s="144"/>
+      <c r="X227" s="141"/>
       <c r="Z227" s="74">
         <v>0</v>
       </c>
@@ -81811,28 +81813,28 @@
       <c r="A228" s="52">
         <v>44049</v>
       </c>
-      <c r="B228" s="142"/>
+      <c r="B228" s="139"/>
       <c r="C228" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D228" s="1"/>
-      <c r="E228" s="143"/>
-      <c r="F228" s="143"/>
+      <c r="E228" s="140"/>
+      <c r="F228" s="140"/>
       <c r="G228" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="H228" s="143"/>
-      <c r="I228" s="143"/>
+      <c r="H228" s="140"/>
+      <c r="I228" s="140"/>
       <c r="J228" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="K228" s="143"/>
-      <c r="L228" s="143"/>
+      <c r="K228" s="140"/>
+      <c r="L228" s="140"/>
       <c r="M228" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="N228" s="143"/>
-      <c r="O228" s="143"/>
+      <c r="N228" s="140"/>
+      <c r="O228" s="140"/>
       <c r="P228" s="1"/>
       <c r="Q228" s="3"/>
       <c r="R228" s="5"/>
@@ -81850,7 +81852,7 @@
         <f t="shared" si="214"/>
         <v>0</v>
       </c>
-      <c r="X228" s="144"/>
+      <c r="X228" s="141"/>
       <c r="Y228" t="s">
         <v>11</v>
       </c>
@@ -81871,28 +81873,28 @@
       <c r="A229" s="52">
         <v>44050</v>
       </c>
-      <c r="B229" s="142"/>
+      <c r="B229" s="139"/>
       <c r="C229" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D229" s="1"/>
-      <c r="E229" s="143"/>
-      <c r="F229" s="143"/>
+      <c r="E229" s="140"/>
+      <c r="F229" s="140"/>
       <c r="G229" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="H229" s="143"/>
-      <c r="I229" s="143"/>
+      <c r="H229" s="140"/>
+      <c r="I229" s="140"/>
       <c r="J229" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="K229" s="143"/>
-      <c r="L229" s="143"/>
+      <c r="K229" s="140"/>
+      <c r="L229" s="140"/>
       <c r="M229" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="N229" s="143"/>
-      <c r="O229" s="143"/>
+      <c r="N229" s="140"/>
+      <c r="O229" s="140"/>
       <c r="P229" s="1"/>
       <c r="Q229" s="3"/>
       <c r="R229" s="5"/>
@@ -81910,7 +81912,7 @@
         <f t="shared" si="214"/>
         <v>0</v>
       </c>
-      <c r="X229" s="144"/>
+      <c r="X229" s="141"/>
       <c r="Y229" s="12">
         <f t="shared" ref="Y229" si="215">SUM(W225:W229)</f>
         <v>4</v>
@@ -81985,7 +81987,7 @@
     <mergeCell ref="K2:O2"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="Z52 Z10 Z59 Z80">
+  <conditionalFormatting sqref="Z10 Z52 Z59 Z80">
     <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -82004,7 +82006,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z38 Z17 Z66 Z87">
+  <conditionalFormatting sqref="Z17 Z38 Z66 Z87">
     <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -82023,7 +82025,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z45 Z24 Z73">
+  <conditionalFormatting sqref="Z24 Z45 Z73">
     <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>